<commit_message>
Update: scoring and serving size files
</commit_message>
<xml_diff>
--- a/dietaryindex_SCORING_ALGORITHM.xlsx
+++ b/dietaryindex_SCORING_ALGORITHM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Desktop/Emory University - Ph.D./dietaryindex_package/dietaryindex/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Desktop/Emory University - Ph.D./dietaryindex_package/dietaryindex publication/Formal_publication/Major revision/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7C8E44-176A-E94D-ADEC-F79BB938D32A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E84E07A8-75EE-424B-A5EF-D180D4B1310A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14280" yWindow="500" windowWidth="21180" windowHeight="19540" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11900" yWindow="2840" windowWidth="26000" windowHeight="19420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HEI2020" sheetId="18" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="494">
   <si>
     <t>Component</t>
   </si>
@@ -837,9 +837,6 @@
   </si>
   <si>
     <t>1. https://www.jandonline.org/article/S0002-8223(09)00288-0/fulltext</t>
-  </si>
-  <si>
-    <t>1. https://academic.oup.com/jn/article/142/6/1009/4688968?login=false</t>
   </si>
   <si>
     <t>1. https://www.fns.usda.gov/healthy-eating-index-hei</t>
@@ -1672,9 +1669,6 @@
     <t>trans fat is not calculated for NHANES given that NHANES does not include it in the nutrition datasets and trans fat concentration in foods is changing every year since 2005 (reference 2)</t>
   </si>
   <si>
-    <t>2. https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4424776/</t>
-  </si>
-  <si>
     <t>From reference 1, table S8 in the supplement</t>
   </si>
   <si>
@@ -1754,6 +1748,12 @@
   </si>
   <si>
     <t>2. https://jamanetwork.com/journals/jamainternalmedicine/fullarticle/413957</t>
+  </si>
+  <si>
+    <t>2. https://www.ncbi.nlm.nih.gov/pmc/articles/PMC3738221/</t>
+  </si>
+  <si>
+    <t>1. https://www.ncbi.nlm.nih.gov/pmc/articles/PMC3738221/</t>
   </si>
 </sst>
 </file>
@@ -2586,31 +2586,160 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2635,140 +2764,11 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3119,8 +3119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184C0948-E756-E040-A146-F3B3FA932BCF}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H17"/>
+    <sheetView topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3136,7 +3136,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="107" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B1" s="107"/>
       <c r="C1" s="107"/>
@@ -3169,7 +3169,7 @@
         <v>30</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -3188,7 +3188,7 @@
     </row>
     <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>16</v>
@@ -3212,7 +3212,7 @@
     </row>
     <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>18</v>
@@ -3236,7 +3236,7 @@
     </row>
     <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>19</v>
@@ -3260,7 +3260,7 @@
     </row>
     <row r="7" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>20</v>
@@ -3284,7 +3284,7 @@
     </row>
     <row r="8" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>22</v>
@@ -3308,7 +3308,7 @@
     </row>
     <row r="9" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>23</v>
@@ -3332,7 +3332,7 @@
     </row>
     <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>6</v>
@@ -3416,7 +3416,7 @@
     </row>
     <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>9</v>
@@ -3464,7 +3464,7 @@
     </row>
     <row r="16" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>11</v>
@@ -3515,7 +3515,7 @@
     </row>
     <row r="19" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="C19" s="9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D19" s="9">
         <v>0</v>
@@ -3531,12 +3531,12 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="26" x14ac:dyDescent="0.3">
       <c r="A23" s="107" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B23" s="107"/>
       <c r="C23" s="107"/>
@@ -3588,7 +3588,7 @@
     </row>
     <row r="26" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>16</v>
@@ -3603,7 +3603,7 @@
         <v>5</v>
       </c>
       <c r="F26" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G26" t="s">
         <v>32</v>
@@ -3612,7 +3612,7 @@
     </row>
     <row r="27" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>18</v>
@@ -3627,7 +3627,7 @@
         <v>5</v>
       </c>
       <c r="F27" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G27" t="s">
         <v>34</v>
@@ -3636,7 +3636,7 @@
     </row>
     <row r="28" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>19</v>
@@ -3651,7 +3651,7 @@
         <v>5</v>
       </c>
       <c r="F28" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G28" t="s">
         <v>35</v>
@@ -3660,7 +3660,7 @@
     </row>
     <row r="29" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>20</v>
@@ -3675,7 +3675,7 @@
         <v>5</v>
       </c>
       <c r="F29" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G29" t="s">
         <v>36</v>
@@ -3684,7 +3684,7 @@
     </row>
     <row r="30" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>22</v>
@@ -3699,7 +3699,7 @@
         <v>5</v>
       </c>
       <c r="F30" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G30" t="s">
         <v>38</v>
@@ -3708,7 +3708,7 @@
     </row>
     <row r="31" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>23</v>
@@ -3723,7 +3723,7 @@
         <v>5</v>
       </c>
       <c r="F31" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G31" t="s">
         <v>39</v>
@@ -3732,7 +3732,7 @@
     </row>
     <row r="32" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>6</v>
@@ -3771,7 +3771,7 @@
         <v>10</v>
       </c>
       <c r="F33" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="G33" t="s">
         <v>33</v>
@@ -3798,7 +3798,7 @@
         <v>66</v>
       </c>
       <c r="G34" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H34" s="106"/>
     </row>
@@ -3816,7 +3816,7 @@
     </row>
     <row r="36" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>9</v>
@@ -3831,10 +3831,10 @@
         <v>10</v>
       </c>
       <c r="F36" t="s">
+        <v>454</v>
+      </c>
+      <c r="G36" t="s">
         <v>455</v>
-      </c>
-      <c r="G36" t="s">
-        <v>456</v>
       </c>
       <c r="H36" s="106"/>
     </row>
@@ -3858,13 +3858,13 @@
         <v>28</v>
       </c>
       <c r="G37" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="H37" s="106"/>
     </row>
     <row r="38" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>11</v>
@@ -3879,10 +3879,10 @@
         <v>10</v>
       </c>
       <c r="F38" t="s">
+        <v>457</v>
+      </c>
+      <c r="G38" t="s">
         <v>458</v>
-      </c>
-      <c r="G38" t="s">
-        <v>459</v>
       </c>
       <c r="H38" s="106"/>
     </row>
@@ -3903,10 +3903,10 @@
         <v>10</v>
       </c>
       <c r="F39" t="s">
+        <v>459</v>
+      </c>
+      <c r="G39" t="s">
         <v>460</v>
-      </c>
-      <c r="G39" t="s">
-        <v>461</v>
       </c>
       <c r="H39" s="106"/>
     </row>
@@ -3915,7 +3915,7 @@
     </row>
     <row r="41" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="C41" s="9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D41" s="9">
         <v>0</v>
@@ -3931,7 +3931,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>
@@ -3950,8 +3950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C05161-9A17-7E4B-8481-331629413469}">
   <dimension ref="A1:Y50"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y6" sqref="Y6"/>
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4028,10 +4028,10 @@
         <v>199</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>444</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="48" x14ac:dyDescent="0.2">
@@ -4093,7 +4093,7 @@
         <v>7.98</v>
       </c>
       <c r="W2" s="9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="X2">
         <v>-8.8699999999999992</v>
@@ -5954,14 +5954,17 @@
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="A50" s="15" t="s">
         <v>246</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A50" r:id="rId1" xr:uid="{77153C7D-286B-BF42-9C1C-FC54EF5E3C26}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5969,8 +5972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60FBCB0-5448-FF4D-B42D-5906F654A994}">
   <dimension ref="A2:F22"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:E14"/>
+    <sheetView topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6180,7 +6183,7 @@
     </row>
     <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C14" s="9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D14" s="9">
         <v>0</v>
@@ -6196,7 +6199,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.2">
@@ -6428,7 +6431,7 @@
     </row>
     <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C14" s="9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D14" s="9">
         <v>0</v>
@@ -6444,7 +6447,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.2">
@@ -6463,8 +6466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C7AD3D-4B0E-3F40-9E23-03DC11FFBC9F}">
   <dimension ref="A1:H103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
@@ -6483,536 +6486,536 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="162" t="s">
+        <v>310</v>
+      </c>
+      <c r="B1" s="77" t="s">
         <v>311</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="C1" s="165" t="s">
         <v>312</v>
       </c>
-      <c r="C1" s="122" t="s">
-        <v>313</v>
-      </c>
-      <c r="D1" s="123"/>
+      <c r="D1" s="166"/>
       <c r="E1" s="23"/>
       <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6" s="25" customFormat="1" ht="31" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="120"/>
+      <c r="A2" s="163"/>
       <c r="B2" s="78" t="s">
-        <v>314</v>
-      </c>
-      <c r="C2" s="124"/>
-      <c r="D2" s="125"/>
+        <v>313</v>
+      </c>
+      <c r="C2" s="167"/>
+      <c r="D2" s="168"/>
       <c r="E2" s="23"/>
       <c r="F2" s="24"/>
     </row>
     <row r="3" spans="1:6" s="29" customFormat="1" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="121"/>
+      <c r="A3" s="164"/>
       <c r="B3" s="26" t="s">
+        <v>314</v>
+      </c>
+      <c r="C3" s="27" t="s">
         <v>315</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="D3" s="28" t="s">
         <v>316</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="E3" s="103" t="s">
         <v>317</v>
       </c>
-      <c r="E3" s="103" t="s">
+      <c r="F3" s="103" t="s">
         <v>318</v>
       </c>
-      <c r="F3" s="103" t="s">
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="169" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="126" t="s">
+      <c r="B4" s="170" t="s">
         <v>320</v>
       </c>
-      <c r="B4" s="128" t="s">
+      <c r="C4" s="137">
+        <v>0</v>
+      </c>
+      <c r="D4" s="30" t="s">
         <v>321</v>
       </c>
-      <c r="C4" s="130">
-        <v>0</v>
-      </c>
-      <c r="D4" s="30" t="s">
+      <c r="E4" s="31" t="s">
         <v>322</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="F4" s="32"/>
+    </row>
+    <row r="5" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="161"/>
+      <c r="B5" s="171"/>
+      <c r="C5" s="160"/>
+      <c r="D5" s="33" t="s">
         <v>323</v>
-      </c>
-      <c r="F4" s="32"/>
-    </row>
-    <row r="5" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="127"/>
-      <c r="B5" s="129"/>
-      <c r="C5" s="131"/>
-      <c r="D5" s="33" t="s">
-        <v>324</v>
       </c>
       <c r="E5" s="31"/>
       <c r="F5" s="32"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="113" t="s">
+      <c r="A6" s="117" t="s">
+        <v>324</v>
+      </c>
+      <c r="B6" s="119" t="s">
         <v>325</v>
       </c>
-      <c r="B6" s="115" t="s">
+      <c r="C6" s="117" t="s">
         <v>326</v>
       </c>
-      <c r="C6" s="113" t="s">
+      <c r="D6" s="157" t="s">
         <v>327</v>
       </c>
-      <c r="D6" s="117" t="s">
+      <c r="E6" s="92" t="s">
         <v>328</v>
-      </c>
-      <c r="E6" s="92" t="s">
-        <v>329</v>
       </c>
       <c r="F6" s="93">
         <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="114"/>
-      <c r="B7" s="116"/>
-      <c r="C7" s="114"/>
-      <c r="D7" s="118"/>
+      <c r="A7" s="144"/>
+      <c r="B7" s="145"/>
+      <c r="C7" s="144"/>
+      <c r="D7" s="158"/>
       <c r="E7" s="94" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F7" s="95">
         <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="114"/>
-      <c r="B8" s="116"/>
-      <c r="C8" s="114"/>
-      <c r="D8" s="118"/>
+      <c r="A8" s="144"/>
+      <c r="B8" s="145"/>
+      <c r="C8" s="144"/>
+      <c r="D8" s="158"/>
       <c r="E8" s="94" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F8" s="95">
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="132" t="s">
+      <c r="A9" s="135" t="s">
+        <v>331</v>
+      </c>
+      <c r="B9" s="137" t="s">
         <v>332</v>
       </c>
-      <c r="B9" s="130" t="s">
+      <c r="C9" s="137">
+        <v>0</v>
+      </c>
+      <c r="D9" s="137" t="s">
         <v>333</v>
       </c>
-      <c r="C9" s="130">
-        <v>0</v>
-      </c>
-      <c r="D9" s="130" t="s">
+      <c r="E9" s="34" t="s">
         <v>334</v>
-      </c>
-      <c r="E9" s="34" t="s">
-        <v>335</v>
       </c>
       <c r="F9" s="35">
         <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="133"/>
-      <c r="B10" s="134"/>
-      <c r="C10" s="134"/>
-      <c r="D10" s="134"/>
+      <c r="A10" s="136"/>
+      <c r="B10" s="138"/>
+      <c r="C10" s="138"/>
+      <c r="D10" s="138"/>
       <c r="E10" s="36" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F10" s="37">
         <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="133"/>
-      <c r="B11" s="134"/>
-      <c r="C11" s="134"/>
-      <c r="D11" s="134"/>
+      <c r="A11" s="136"/>
+      <c r="B11" s="138"/>
+      <c r="C11" s="138"/>
+      <c r="D11" s="138"/>
       <c r="E11" s="36" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F11" s="37">
         <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="133"/>
-      <c r="B12" s="134"/>
-      <c r="C12" s="134"/>
-      <c r="D12" s="134"/>
+      <c r="A12" s="136"/>
+      <c r="B12" s="138"/>
+      <c r="C12" s="138"/>
+      <c r="D12" s="138"/>
       <c r="E12" s="36"/>
       <c r="F12" s="37"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="133"/>
-      <c r="B13" s="134"/>
-      <c r="C13" s="134"/>
-      <c r="D13" s="134"/>
+      <c r="A13" s="136"/>
+      <c r="B13" s="138"/>
+      <c r="C13" s="138"/>
+      <c r="D13" s="138"/>
       <c r="E13" s="36" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F13" s="37">
         <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="133"/>
-      <c r="B14" s="134"/>
-      <c r="C14" s="134"/>
-      <c r="D14" s="134"/>
+      <c r="A14" s="136"/>
+      <c r="B14" s="138"/>
+      <c r="C14" s="138"/>
+      <c r="D14" s="138"/>
       <c r="E14" s="36" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F14" s="37">
         <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="133"/>
-      <c r="B15" s="134"/>
-      <c r="C15" s="134"/>
-      <c r="D15" s="134"/>
+      <c r="A15" s="136"/>
+      <c r="B15" s="138"/>
+      <c r="C15" s="138"/>
+      <c r="D15" s="138"/>
       <c r="E15" s="36" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F15" s="37">
         <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="133"/>
-      <c r="B16" s="134"/>
-      <c r="C16" s="134"/>
-      <c r="D16" s="134"/>
+      <c r="A16" s="136"/>
+      <c r="B16" s="138"/>
+      <c r="C16" s="138"/>
+      <c r="D16" s="138"/>
       <c r="E16" s="36" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F16" s="37">
         <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="133"/>
-      <c r="B17" s="134"/>
-      <c r="C17" s="134"/>
-      <c r="D17" s="134"/>
+      <c r="A17" s="136"/>
+      <c r="B17" s="138"/>
+      <c r="C17" s="138"/>
+      <c r="D17" s="138"/>
       <c r="E17" s="36" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F17" s="37">
         <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="133"/>
-      <c r="B18" s="134"/>
-      <c r="C18" s="134"/>
-      <c r="D18" s="134"/>
+      <c r="A18" s="136"/>
+      <c r="B18" s="138"/>
+      <c r="C18" s="138"/>
+      <c r="D18" s="138"/>
       <c r="E18" s="36" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F18" s="37">
         <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="133"/>
-      <c r="B19" s="134"/>
-      <c r="C19" s="134"/>
-      <c r="D19" s="134"/>
+      <c r="A19" s="136"/>
+      <c r="B19" s="138"/>
+      <c r="C19" s="138"/>
+      <c r="D19" s="138"/>
       <c r="E19" s="36" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F19" s="37">
         <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="133"/>
-      <c r="B20" s="134"/>
-      <c r="C20" s="134"/>
-      <c r="D20" s="134"/>
+      <c r="A20" s="136"/>
+      <c r="B20" s="138"/>
+      <c r="C20" s="138"/>
+      <c r="D20" s="138"/>
       <c r="E20" s="36" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F20" s="37">
         <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="133"/>
-      <c r="B21" s="134"/>
-      <c r="C21" s="134"/>
-      <c r="D21" s="134"/>
+      <c r="A21" s="136"/>
+      <c r="B21" s="138"/>
+      <c r="C21" s="138"/>
+      <c r="D21" s="138"/>
       <c r="E21" s="36" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F21" s="38">
         <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="133"/>
-      <c r="B22" s="134"/>
-      <c r="C22" s="134"/>
-      <c r="D22" s="134"/>
+      <c r="A22" s="136"/>
+      <c r="B22" s="138"/>
+      <c r="C22" s="138"/>
+      <c r="D22" s="138"/>
       <c r="E22" s="36" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F22" s="38">
         <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="133"/>
-      <c r="B23" s="134"/>
-      <c r="C23" s="134"/>
-      <c r="D23" s="134"/>
+      <c r="A23" s="136"/>
+      <c r="B23" s="138"/>
+      <c r="C23" s="138"/>
+      <c r="D23" s="138"/>
       <c r="E23" s="36" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F23" s="38">
         <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="133"/>
-      <c r="B24" s="134"/>
-      <c r="C24" s="134"/>
-      <c r="D24" s="134"/>
+      <c r="A24" s="136"/>
+      <c r="B24" s="138"/>
+      <c r="C24" s="138"/>
+      <c r="D24" s="138"/>
       <c r="E24" s="36" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F24" s="37">
         <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="133"/>
-      <c r="B25" s="134"/>
-      <c r="C25" s="134"/>
-      <c r="D25" s="134"/>
+      <c r="A25" s="136"/>
+      <c r="B25" s="138"/>
+      <c r="C25" s="138"/>
+      <c r="D25" s="138"/>
       <c r="E25" s="36" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F25" s="37">
         <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="133"/>
-      <c r="B26" s="134"/>
-      <c r="C26" s="134"/>
-      <c r="D26" s="134"/>
+      <c r="A26" s="136"/>
+      <c r="B26" s="138"/>
+      <c r="C26" s="138"/>
+      <c r="D26" s="138"/>
       <c r="E26" s="36" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F26" s="37">
         <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="133"/>
-      <c r="B27" s="134"/>
-      <c r="C27" s="134"/>
-      <c r="D27" s="134"/>
+      <c r="A27" s="136"/>
+      <c r="B27" s="138"/>
+      <c r="C27" s="138"/>
+      <c r="D27" s="138"/>
       <c r="E27" s="36" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F27" s="37">
         <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="133"/>
-      <c r="B28" s="134"/>
-      <c r="C28" s="134"/>
-      <c r="D28" s="134"/>
+      <c r="A28" s="136"/>
+      <c r="B28" s="138"/>
+      <c r="C28" s="138"/>
+      <c r="D28" s="138"/>
       <c r="E28" s="36" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F28" s="37">
         <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="133"/>
-      <c r="B29" s="134"/>
-      <c r="C29" s="134"/>
-      <c r="D29" s="134"/>
+      <c r="A29" s="136"/>
+      <c r="B29" s="138"/>
+      <c r="C29" s="138"/>
+      <c r="D29" s="138"/>
       <c r="E29" s="36" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F29" s="37">
         <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="133"/>
-      <c r="B30" s="134"/>
-      <c r="C30" s="134"/>
-      <c r="D30" s="134"/>
+      <c r="A30" s="136"/>
+      <c r="B30" s="138"/>
+      <c r="C30" s="138"/>
+      <c r="D30" s="138"/>
       <c r="E30" s="36" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F30" s="37">
         <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="133"/>
-      <c r="B31" s="134"/>
-      <c r="C31" s="134"/>
-      <c r="D31" s="134"/>
+      <c r="A31" s="136"/>
+      <c r="B31" s="138"/>
+      <c r="C31" s="138"/>
+      <c r="D31" s="138"/>
       <c r="E31" s="36" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F31" s="37">
         <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="133"/>
-      <c r="B32" s="134"/>
-      <c r="C32" s="134"/>
-      <c r="D32" s="134"/>
+      <c r="A32" s="136"/>
+      <c r="B32" s="138"/>
+      <c r="C32" s="138"/>
+      <c r="D32" s="138"/>
       <c r="E32" s="36" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F32" s="37">
         <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="133"/>
-      <c r="B33" s="134"/>
-      <c r="C33" s="134"/>
-      <c r="D33" s="134"/>
+      <c r="A33" s="136"/>
+      <c r="B33" s="138"/>
+      <c r="C33" s="138"/>
+      <c r="D33" s="138"/>
       <c r="E33" s="36" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F33" s="38">
         <v>37.5</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="133"/>
-      <c r="B34" s="134"/>
-      <c r="C34" s="134"/>
-      <c r="D34" s="134"/>
+      <c r="A34" s="136"/>
+      <c r="B34" s="138"/>
+      <c r="C34" s="138"/>
+      <c r="D34" s="138"/>
       <c r="E34" s="36"/>
       <c r="F34" s="38"/>
       <c r="G34" s="8"/>
       <c r="H34" s="39"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="133"/>
-      <c r="B35" s="134"/>
-      <c r="C35" s="134"/>
-      <c r="D35" s="134"/>
+      <c r="A35" s="136"/>
+      <c r="B35" s="138"/>
+      <c r="C35" s="138"/>
+      <c r="D35" s="138"/>
       <c r="E35" s="36" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F35" s="38">
         <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="133"/>
-      <c r="B36" s="134"/>
-      <c r="C36" s="134"/>
-      <c r="D36" s="134"/>
+      <c r="A36" s="136"/>
+      <c r="B36" s="138"/>
+      <c r="C36" s="138"/>
+      <c r="D36" s="138"/>
       <c r="E36" s="36"/>
       <c r="F36" s="38"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="133"/>
-      <c r="B37" s="134"/>
-      <c r="C37" s="134"/>
-      <c r="D37" s="134"/>
+      <c r="A37" s="136"/>
+      <c r="B37" s="138"/>
+      <c r="C37" s="138"/>
+      <c r="D37" s="138"/>
       <c r="E37" s="36" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F37" s="37">
         <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="133"/>
-      <c r="B38" s="134"/>
-      <c r="C38" s="134"/>
-      <c r="D38" s="134"/>
+      <c r="A38" s="136"/>
+      <c r="B38" s="138"/>
+      <c r="C38" s="138"/>
+      <c r="D38" s="138"/>
       <c r="E38" s="36" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F38" s="37">
         <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="127"/>
-      <c r="B39" s="131"/>
-      <c r="C39" s="131"/>
-      <c r="D39" s="131"/>
+      <c r="A39" s="161"/>
+      <c r="B39" s="160"/>
+      <c r="C39" s="160"/>
+      <c r="D39" s="160"/>
       <c r="E39" s="40" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F39" s="41">
         <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="132" t="s">
+      <c r="A40" s="135" t="s">
+        <v>362</v>
+      </c>
+      <c r="B40" s="137" t="s">
         <v>363</v>
       </c>
-      <c r="B40" s="130" t="s">
+      <c r="C40" s="137">
+        <v>0</v>
+      </c>
+      <c r="D40" s="137" t="s">
         <v>364</v>
       </c>
-      <c r="C40" s="130">
-        <v>0</v>
-      </c>
-      <c r="D40" s="130" t="s">
+      <c r="E40" s="42" t="s">
         <v>365</v>
-      </c>
-      <c r="E40" s="42" t="s">
-        <v>366</v>
       </c>
       <c r="F40" s="43">
         <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="133"/>
-      <c r="B41" s="134"/>
-      <c r="C41" s="134"/>
-      <c r="D41" s="134"/>
+      <c r="A41" s="136"/>
+      <c r="B41" s="138"/>
+      <c r="C41" s="138"/>
+      <c r="D41" s="138"/>
       <c r="E41" s="44"/>
       <c r="F41" s="45"/>
     </row>
     <row r="42" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="133"/>
-      <c r="B42" s="134"/>
-      <c r="C42" s="134"/>
-      <c r="D42" s="134"/>
+      <c r="A42" s="136"/>
+      <c r="B42" s="138"/>
+      <c r="C42" s="138"/>
+      <c r="D42" s="138"/>
       <c r="E42" s="44" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F42" s="37">
         <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="133"/>
-      <c r="B43" s="134"/>
-      <c r="C43" s="134"/>
-      <c r="D43" s="134"/>
+      <c r="A43" s="136"/>
+      <c r="B43" s="138"/>
+      <c r="C43" s="138"/>
+      <c r="D43" s="138"/>
       <c r="E43" s="44" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F43" s="37">
         <v>114</v>
@@ -7020,11 +7023,11 @@
     </row>
     <row r="44" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="30"/>
-      <c r="B44" s="134"/>
-      <c r="C44" s="134"/>
-      <c r="D44" s="134"/>
+      <c r="B44" s="138"/>
+      <c r="C44" s="138"/>
+      <c r="D44" s="138"/>
       <c r="E44" s="44" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F44" s="37">
         <v>135</v>
@@ -7032,11 +7035,11 @@
     </row>
     <row r="45" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="30"/>
-      <c r="B45" s="134"/>
-      <c r="C45" s="134"/>
-      <c r="D45" s="134"/>
+      <c r="B45" s="138"/>
+      <c r="C45" s="138"/>
+      <c r="D45" s="138"/>
       <c r="E45" s="44" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F45" s="45">
         <v>100.5</v>
@@ -7044,11 +7047,11 @@
     </row>
     <row r="46" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="30"/>
-      <c r="B46" s="134"/>
-      <c r="C46" s="134"/>
-      <c r="D46" s="134"/>
+      <c r="B46" s="138"/>
+      <c r="C46" s="138"/>
+      <c r="D46" s="138"/>
       <c r="E46" s="44" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F46" s="45">
         <v>138</v>
@@ -7056,11 +7059,11 @@
     </row>
     <row r="47" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="30"/>
-      <c r="B47" s="134"/>
-      <c r="C47" s="134"/>
-      <c r="D47" s="134"/>
+      <c r="B47" s="138"/>
+      <c r="C47" s="138"/>
+      <c r="D47" s="138"/>
       <c r="E47" s="44" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F47" s="45">
         <v>166</v>
@@ -7068,11 +7071,11 @@
     </row>
     <row r="48" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="30"/>
-      <c r="B48" s="134"/>
-      <c r="C48" s="134"/>
-      <c r="D48" s="134"/>
+      <c r="B48" s="138"/>
+      <c r="C48" s="138"/>
+      <c r="D48" s="138"/>
       <c r="E48" s="44" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F48" s="45">
         <v>127.5</v>
@@ -7080,19 +7083,19 @@
     </row>
     <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="30"/>
-      <c r="B49" s="134"/>
-      <c r="C49" s="134"/>
-      <c r="D49" s="134"/>
+      <c r="B49" s="138"/>
+      <c r="C49" s="138"/>
+      <c r="D49" s="138"/>
       <c r="E49" s="44"/>
       <c r="F49" s="45"/>
     </row>
     <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="30"/>
-      <c r="B50" s="134"/>
-      <c r="C50" s="134"/>
-      <c r="D50" s="134"/>
+      <c r="B50" s="138"/>
+      <c r="C50" s="138"/>
+      <c r="D50" s="138"/>
       <c r="E50" s="44" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F50" s="37">
         <v>131</v>
@@ -7100,11 +7103,11 @@
     </row>
     <row r="51" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="30"/>
-      <c r="B51" s="134"/>
-      <c r="C51" s="134"/>
-      <c r="D51" s="134"/>
+      <c r="B51" s="138"/>
+      <c r="C51" s="138"/>
+      <c r="D51" s="138"/>
       <c r="E51" s="44" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F51" s="37">
         <v>120</v>
@@ -7112,11 +7115,11 @@
     </row>
     <row r="52" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="30"/>
-      <c r="B52" s="134"/>
-      <c r="C52" s="134"/>
-      <c r="D52" s="134"/>
+      <c r="B52" s="138"/>
+      <c r="C52" s="138"/>
+      <c r="D52" s="138"/>
       <c r="E52" s="44" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F52" s="37">
         <v>75</v>
@@ -7124,11 +7127,11 @@
     </row>
     <row r="53" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="30"/>
-      <c r="B53" s="134"/>
-      <c r="C53" s="134"/>
-      <c r="D53" s="134"/>
+      <c r="B53" s="138"/>
+      <c r="C53" s="138"/>
+      <c r="D53" s="138"/>
       <c r="E53" s="44" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F53" s="37">
         <v>73</v>
@@ -7136,11 +7139,11 @@
     </row>
     <row r="54" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="30"/>
-      <c r="B54" s="134"/>
-      <c r="C54" s="134"/>
-      <c r="D54" s="134"/>
+      <c r="B54" s="138"/>
+      <c r="C54" s="138"/>
+      <c r="D54" s="138"/>
       <c r="E54" s="44" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F54" s="37">
         <v>128</v>
@@ -7148,19 +7151,19 @@
     </row>
     <row r="55" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="30"/>
-      <c r="B55" s="134"/>
-      <c r="C55" s="134"/>
-      <c r="D55" s="134"/>
+      <c r="B55" s="138"/>
+      <c r="C55" s="138"/>
+      <c r="D55" s="138"/>
       <c r="E55" s="44"/>
       <c r="F55" s="37"/>
     </row>
     <row r="56" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="30"/>
-      <c r="B56" s="134"/>
-      <c r="C56" s="134"/>
-      <c r="D56" s="134"/>
+      <c r="B56" s="138"/>
+      <c r="C56" s="138"/>
+      <c r="D56" s="138"/>
       <c r="E56" s="44" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F56" s="37">
         <v>241</v>
@@ -7168,27 +7171,27 @@
     </row>
     <row r="57" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="30"/>
-      <c r="B57" s="134"/>
-      <c r="C57" s="134"/>
-      <c r="D57" s="134"/>
+      <c r="B57" s="138"/>
+      <c r="C57" s="138"/>
+      <c r="D57" s="138"/>
       <c r="E57" s="44"/>
       <c r="F57" s="45"/>
     </row>
     <row r="58" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="30"/>
-      <c r="B58" s="134"/>
-      <c r="C58" s="134"/>
-      <c r="D58" s="134"/>
+      <c r="B58" s="138"/>
+      <c r="C58" s="138"/>
+      <c r="D58" s="138"/>
       <c r="E58" s="44"/>
       <c r="F58" s="45"/>
     </row>
     <row r="59" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="30"/>
-      <c r="B59" s="134"/>
-      <c r="C59" s="134"/>
-      <c r="D59" s="134"/>
+      <c r="B59" s="138"/>
+      <c r="C59" s="138"/>
+      <c r="D59" s="138"/>
       <c r="E59" s="44" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F59" s="45">
         <v>128</v>
@@ -7196,11 +7199,11 @@
     </row>
     <row r="60" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="30"/>
-      <c r="B60" s="134"/>
-      <c r="C60" s="134"/>
-      <c r="D60" s="134"/>
+      <c r="B60" s="138"/>
+      <c r="C60" s="138"/>
+      <c r="D60" s="138"/>
       <c r="E60" s="44" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F60" s="45">
         <v>127</v>
@@ -7208,11 +7211,11 @@
     </row>
     <row r="61" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="30"/>
-      <c r="B61" s="134"/>
-      <c r="C61" s="134"/>
-      <c r="D61" s="134"/>
+      <c r="B61" s="138"/>
+      <c r="C61" s="138"/>
+      <c r="D61" s="138"/>
       <c r="E61" s="44" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F61" s="45">
         <v>128</v>
@@ -7220,502 +7223,502 @@
     </row>
     <row r="62" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="30"/>
-      <c r="B62" s="134"/>
-      <c r="C62" s="134"/>
-      <c r="D62" s="134"/>
+      <c r="B62" s="138"/>
+      <c r="C62" s="138"/>
+      <c r="D62" s="138"/>
       <c r="E62" s="44"/>
       <c r="F62" s="45"/>
     </row>
     <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="30"/>
-      <c r="B63" s="134"/>
-      <c r="C63" s="134"/>
-      <c r="D63" s="134"/>
+      <c r="B63" s="138"/>
+      <c r="C63" s="138"/>
+      <c r="D63" s="138"/>
       <c r="E63" s="44"/>
       <c r="F63" s="45"/>
     </row>
     <row r="64" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="30"/>
-      <c r="B64" s="131"/>
-      <c r="C64" s="131"/>
-      <c r="D64" s="131"/>
+      <c r="B64" s="160"/>
+      <c r="C64" s="160"/>
+      <c r="D64" s="160"/>
       <c r="E64" s="46"/>
       <c r="F64" s="47"/>
     </row>
     <row r="65" spans="1:6" s="48" customFormat="1" ht="149.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="79" t="s">
+        <v>382</v>
+      </c>
+      <c r="B65" s="80" t="s">
         <v>383</v>
       </c>
-      <c r="B65" s="80" t="s">
+      <c r="C65" s="80" t="s">
         <v>384</v>
       </c>
-      <c r="C65" s="80" t="s">
+      <c r="D65" s="91" t="s">
         <v>385</v>
       </c>
-      <c r="D65" s="91" t="s">
+      <c r="E65" s="152" t="s">
         <v>386</v>
       </c>
-      <c r="E65" s="135" t="s">
+      <c r="F65" s="153"/>
+    </row>
+    <row r="66" spans="1:6" ht="29.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="117" t="s">
         <v>387</v>
       </c>
-      <c r="F65" s="136"/>
-    </row>
-    <row r="66" spans="1:6" ht="29.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="113" t="s">
+      <c r="B66" s="119" t="s">
         <v>388</v>
       </c>
-      <c r="B66" s="115" t="s">
+      <c r="C66" s="154" t="s">
         <v>389</v>
       </c>
-      <c r="C66" s="139" t="s">
+      <c r="D66" s="157" t="s">
         <v>390</v>
       </c>
-      <c r="D66" s="117" t="s">
+      <c r="E66" s="49" t="s">
         <v>391</v>
-      </c>
-      <c r="E66" s="49" t="s">
-        <v>392</v>
       </c>
       <c r="F66" s="50">
         <v>45</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" s="114"/>
-      <c r="B67" s="116"/>
-      <c r="C67" s="140"/>
-      <c r="D67" s="118"/>
+      <c r="A67" s="144"/>
+      <c r="B67" s="145"/>
+      <c r="C67" s="155"/>
+      <c r="D67" s="158"/>
       <c r="E67" s="51"/>
       <c r="F67" s="52"/>
     </row>
     <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A68" s="114"/>
-      <c r="B68" s="116"/>
-      <c r="C68" s="140"/>
-      <c r="D68" s="118"/>
+      <c r="A68" s="144"/>
+      <c r="B68" s="145"/>
+      <c r="C68" s="155"/>
+      <c r="D68" s="158"/>
       <c r="E68" s="51" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F68" s="52">
         <v>13</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A69" s="114"/>
-      <c r="B69" s="116"/>
-      <c r="C69" s="140"/>
-      <c r="D69" s="118"/>
+      <c r="A69" s="144"/>
+      <c r="B69" s="145"/>
+      <c r="C69" s="155"/>
+      <c r="D69" s="158"/>
       <c r="E69" s="51"/>
       <c r="F69" s="52"/>
     </row>
     <row r="70" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A70" s="114"/>
-      <c r="B70" s="116"/>
-      <c r="C70" s="140"/>
-      <c r="D70" s="118"/>
+      <c r="A70" s="144"/>
+      <c r="B70" s="145"/>
+      <c r="C70" s="155"/>
+      <c r="D70" s="158"/>
       <c r="E70" s="51" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F70" s="52">
         <v>27</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A71" s="114"/>
-      <c r="B71" s="116"/>
-      <c r="C71" s="140"/>
-      <c r="D71" s="118"/>
+      <c r="A71" s="144"/>
+      <c r="B71" s="145"/>
+      <c r="C71" s="155"/>
+      <c r="D71" s="158"/>
       <c r="E71" s="51" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F71" s="52">
         <v>85</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A72" s="114"/>
-      <c r="B72" s="116"/>
-      <c r="C72" s="140"/>
-      <c r="D72" s="118"/>
+      <c r="A72" s="144"/>
+      <c r="B72" s="145"/>
+      <c r="C72" s="155"/>
+      <c r="D72" s="158"/>
       <c r="E72" s="51"/>
       <c r="F72" s="52"/>
     </row>
     <row r="73" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A73" s="114"/>
-      <c r="B73" s="116"/>
-      <c r="C73" s="140"/>
-      <c r="D73" s="118"/>
+      <c r="A73" s="144"/>
+      <c r="B73" s="145"/>
+      <c r="C73" s="155"/>
+      <c r="D73" s="158"/>
       <c r="E73" s="51" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F73" s="52">
         <v>85.4</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A74" s="114"/>
-      <c r="B74" s="116"/>
-      <c r="C74" s="140"/>
-      <c r="D74" s="118"/>
+      <c r="A74" s="144"/>
+      <c r="B74" s="145"/>
+      <c r="C74" s="155"/>
+      <c r="D74" s="158"/>
       <c r="E74" s="51"/>
       <c r="F74" s="52"/>
     </row>
     <row r="75" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="137"/>
-      <c r="B75" s="138"/>
-      <c r="C75" s="141"/>
-      <c r="D75" s="142"/>
+      <c r="A75" s="118"/>
+      <c r="B75" s="120"/>
+      <c r="C75" s="156"/>
+      <c r="D75" s="159"/>
       <c r="E75" s="53" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F75" s="54">
         <v>140</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="29.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="113" t="s">
+      <c r="A76" s="117" t="s">
+        <v>397</v>
+      </c>
+      <c r="B76" s="119" t="s">
         <v>398</v>
       </c>
-      <c r="B76" s="115" t="s">
+      <c r="C76" s="149" t="s">
+        <v>389</v>
+      </c>
+      <c r="D76" s="146" t="s">
         <v>399</v>
-      </c>
-      <c r="C76" s="146" t="s">
-        <v>390</v>
-      </c>
-      <c r="D76" s="143" t="s">
-        <v>400</v>
       </c>
       <c r="E76" s="81"/>
       <c r="F76" s="82"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="114"/>
-      <c r="B77" s="116"/>
-      <c r="C77" s="147"/>
-      <c r="D77" s="144"/>
+      <c r="A77" s="144"/>
+      <c r="B77" s="145"/>
+      <c r="C77" s="150"/>
+      <c r="D77" s="147"/>
       <c r="E77" s="83" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F77" s="84">
         <v>140</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="137"/>
-      <c r="B78" s="138"/>
-      <c r="C78" s="148"/>
-      <c r="D78" s="145"/>
+      <c r="A78" s="118"/>
+      <c r="B78" s="120"/>
+      <c r="C78" s="151"/>
+      <c r="D78" s="148"/>
       <c r="E78" s="85" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F78" s="86">
         <v>140</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="113" t="s">
+      <c r="A79" s="117" t="s">
+        <v>402</v>
+      </c>
+      <c r="B79" s="119" t="s">
         <v>403</v>
       </c>
-      <c r="B79" s="115" t="s">
+      <c r="C79" s="119" t="s">
         <v>404</v>
       </c>
-      <c r="C79" s="115" t="s">
+      <c r="D79" s="146" t="s">
         <v>405</v>
       </c>
-      <c r="D79" s="143" t="s">
+      <c r="E79" s="87" t="s">
         <v>406</v>
-      </c>
-      <c r="E79" s="87" t="s">
-        <v>407</v>
       </c>
       <c r="F79" s="88">
         <v>50</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="114"/>
-      <c r="B80" s="116"/>
-      <c r="C80" s="116"/>
-      <c r="D80" s="144"/>
+      <c r="A80" s="144"/>
+      <c r="B80" s="145"/>
+      <c r="C80" s="145"/>
+      <c r="D80" s="147"/>
       <c r="E80" s="83"/>
       <c r="F80" s="89"/>
     </row>
     <row r="81" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="137"/>
-      <c r="B81" s="138"/>
-      <c r="C81" s="138"/>
-      <c r="D81" s="145"/>
+      <c r="A81" s="118"/>
+      <c r="B81" s="120"/>
+      <c r="C81" s="120"/>
+      <c r="D81" s="148"/>
       <c r="E81" s="85"/>
       <c r="F81" s="90"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A82" s="149" t="s">
+      <c r="A82" s="127" t="s">
+        <v>407</v>
+      </c>
+      <c r="B82" s="131" t="s">
         <v>408</v>
       </c>
-      <c r="B82" s="151" t="s">
+      <c r="C82" s="141">
+        <v>0</v>
+      </c>
+      <c r="D82" s="141" t="s">
         <v>409</v>
       </c>
-      <c r="C82" s="153">
-        <v>0</v>
-      </c>
-      <c r="D82" s="153" t="s">
+      <c r="E82" s="96" t="s">
         <v>410</v>
-      </c>
-      <c r="E82" s="96" t="s">
-        <v>411</v>
       </c>
       <c r="F82" s="97">
         <v>98</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A83" s="150"/>
-      <c r="B83" s="152"/>
-      <c r="C83" s="154"/>
-      <c r="D83" s="154"/>
+      <c r="A83" s="139"/>
+      <c r="B83" s="140"/>
+      <c r="C83" s="142"/>
+      <c r="D83" s="142"/>
       <c r="E83" s="98"/>
       <c r="F83" s="99"/>
       <c r="G83" s="55"/>
     </row>
     <row r="84" spans="1:7" s="56" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="150"/>
-      <c r="B84" s="152"/>
-      <c r="C84" s="154"/>
-      <c r="D84" s="154"/>
+      <c r="A84" s="139"/>
+      <c r="B84" s="140"/>
+      <c r="C84" s="142"/>
+      <c r="D84" s="142"/>
       <c r="E84" s="98" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F84" s="99">
         <v>85</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A85" s="150"/>
-      <c r="B85" s="152"/>
-      <c r="C85" s="154"/>
-      <c r="D85" s="154"/>
+      <c r="A85" s="139"/>
+      <c r="B85" s="140"/>
+      <c r="C85" s="142"/>
+      <c r="D85" s="142"/>
       <c r="E85" s="98" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F85" s="99">
         <v>111.32</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="150"/>
-      <c r="B86" s="152"/>
-      <c r="C86" s="154"/>
-      <c r="D86" s="155"/>
+      <c r="A86" s="139"/>
+      <c r="B86" s="140"/>
+      <c r="C86" s="142"/>
+      <c r="D86" s="143"/>
       <c r="E86" s="100" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F86" s="101">
         <v>112.2</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="43.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="132" t="s">
+      <c r="A87" s="135" t="s">
+        <v>414</v>
+      </c>
+      <c r="B87" s="135" t="s">
         <v>415</v>
       </c>
-      <c r="B87" s="132" t="s">
+      <c r="C87" s="137">
+        <v>0</v>
+      </c>
+      <c r="D87" s="137" t="s">
         <v>416</v>
       </c>
-      <c r="C87" s="130">
-        <v>0</v>
-      </c>
-      <c r="D87" s="130" t="s">
+      <c r="E87" s="57" t="s">
         <v>417</v>
-      </c>
-      <c r="E87" s="57" t="s">
-        <v>418</v>
       </c>
       <c r="F87" s="58">
         <v>16</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A88" s="133"/>
-      <c r="B88" s="133"/>
-      <c r="C88" s="134"/>
-      <c r="D88" s="134"/>
+      <c r="A88" s="136"/>
+      <c r="B88" s="136"/>
+      <c r="C88" s="138"/>
+      <c r="D88" s="138"/>
       <c r="E88" s="59" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F88" s="60">
         <v>28</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A89" s="133"/>
-      <c r="B89" s="133"/>
-      <c r="C89" s="134"/>
-      <c r="D89" s="134"/>
+      <c r="A89" s="136"/>
+      <c r="B89" s="136"/>
+      <c r="C89" s="138"/>
+      <c r="D89" s="138"/>
       <c r="E89" s="59"/>
       <c r="F89" s="60"/>
     </row>
     <row r="90" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A90" s="133"/>
-      <c r="B90" s="133"/>
-      <c r="C90" s="134"/>
-      <c r="D90" s="134"/>
+      <c r="A90" s="136"/>
+      <c r="B90" s="136"/>
+      <c r="C90" s="138"/>
+      <c r="D90" s="138"/>
       <c r="E90" s="61" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F90" s="62">
         <v>28.4</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="133"/>
-      <c r="B91" s="133"/>
-      <c r="C91" s="134"/>
-      <c r="D91" s="134"/>
+      <c r="A91" s="136"/>
+      <c r="B91" s="136"/>
+      <c r="C91" s="138"/>
+      <c r="D91" s="138"/>
       <c r="E91" s="61"/>
       <c r="F91" s="62"/>
     </row>
     <row r="92" spans="1:7" ht="94" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A92" s="63" t="s">
+        <v>425</v>
+      </c>
+      <c r="B92" s="64" t="s">
         <v>426</v>
       </c>
-      <c r="B92" s="64" t="s">
+      <c r="C92" s="64" t="s">
         <v>427</v>
       </c>
-      <c r="C92" s="64" t="s">
+      <c r="D92" s="69" t="s">
         <v>428</v>
       </c>
-      <c r="D92" s="69" t="s">
+      <c r="E92" s="70" t="s">
         <v>429</v>
       </c>
-      <c r="E92" s="70" t="s">
+      <c r="F92" s="71"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A93" s="117" t="s">
         <v>430</v>
       </c>
-      <c r="F92" s="71"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A93" s="113" t="s">
+      <c r="B93" s="119" t="s">
         <v>431</v>
       </c>
-      <c r="B93" s="115" t="s">
+      <c r="C93" s="119" t="s">
         <v>432</v>
       </c>
-      <c r="C93" s="115" t="s">
+      <c r="D93" s="119" t="s">
         <v>433</v>
       </c>
-      <c r="D93" s="115" t="s">
+      <c r="E93" s="113" t="s">
         <v>434</v>
       </c>
-      <c r="E93" s="168" t="s">
+      <c r="F93" s="114"/>
+    </row>
+    <row r="94" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="118"/>
+      <c r="B94" s="120"/>
+      <c r="C94" s="120"/>
+      <c r="D94" s="120"/>
+      <c r="E94" s="115"/>
+      <c r="F94" s="116"/>
+    </row>
+    <row r="95" spans="1:7" ht="29.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="117" t="s">
         <v>435</v>
       </c>
-      <c r="F93" s="169"/>
-    </row>
-    <row r="94" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="137"/>
-      <c r="B94" s="138"/>
-      <c r="C94" s="138"/>
-      <c r="D94" s="138"/>
-      <c r="E94" s="170"/>
-      <c r="F94" s="171"/>
-    </row>
-    <row r="95" spans="1:7" ht="29.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="113" t="s">
+      <c r="B95" s="119" t="s">
         <v>436</v>
       </c>
-      <c r="B95" s="115" t="s">
+      <c r="C95" s="119" t="s">
         <v>437</v>
       </c>
-      <c r="C95" s="115" t="s">
+      <c r="D95" s="119" t="s">
         <v>438</v>
       </c>
-      <c r="D95" s="115" t="s">
+      <c r="E95" s="72" t="s">
         <v>439</v>
       </c>
-      <c r="E95" s="72" t="s">
+      <c r="F95" s="73"/>
+    </row>
+    <row r="96" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="118"/>
+      <c r="B96" s="120"/>
+      <c r="C96" s="120"/>
+      <c r="D96" s="120"/>
+      <c r="E96" s="74" t="s">
         <v>440</v>
-      </c>
-      <c r="F95" s="73"/>
-    </row>
-    <row r="96" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="137"/>
-      <c r="B96" s="138"/>
-      <c r="C96" s="138"/>
-      <c r="D96" s="138"/>
-      <c r="E96" s="74" t="s">
-        <v>441</v>
       </c>
       <c r="F96" s="75"/>
     </row>
     <row r="97" spans="1:6" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A97" s="102" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B97" s="26" t="s">
+        <v>314</v>
+      </c>
+      <c r="C97" s="27" t="s">
         <v>315</v>
       </c>
-      <c r="C97" s="27" t="s">
-        <v>316</v>
-      </c>
       <c r="D97" s="28" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E97" s="103" t="s">
+        <v>317</v>
+      </c>
+      <c r="F97" s="103" t="s">
         <v>318</v>
       </c>
-      <c r="F97" s="103" t="s">
-        <v>319</v>
-      </c>
     </row>
     <row r="98" spans="1:6" ht="43.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="149" t="s">
+      <c r="A98" s="127" t="s">
+        <v>420</v>
+      </c>
+      <c r="B98" s="129" t="s">
+        <v>325</v>
+      </c>
+      <c r="C98" s="131">
+        <v>0</v>
+      </c>
+      <c r="D98" s="133">
+        <v>100</v>
+      </c>
+      <c r="E98" s="57" t="s">
         <v>421</v>
-      </c>
-      <c r="B98" s="163" t="s">
-        <v>326</v>
-      </c>
-      <c r="C98" s="151">
-        <v>0</v>
-      </c>
-      <c r="D98" s="166">
-        <v>100</v>
-      </c>
-      <c r="E98" s="57" t="s">
-        <v>422</v>
       </c>
       <c r="F98" s="58">
         <v>131</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="162"/>
-      <c r="B99" s="164"/>
-      <c r="C99" s="165"/>
-      <c r="D99" s="167"/>
+      <c r="A99" s="128"/>
+      <c r="B99" s="130"/>
+      <c r="C99" s="132"/>
+      <c r="D99" s="134"/>
       <c r="E99" s="65"/>
       <c r="F99" s="66"/>
     </row>
     <row r="100" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="156" t="s">
+      <c r="A100" s="121" t="s">
+        <v>422</v>
+      </c>
+      <c r="B100" s="121" t="s">
         <v>423</v>
       </c>
-      <c r="B100" s="156" t="s">
-        <v>424</v>
-      </c>
-      <c r="C100" s="158">
-        <v>0</v>
-      </c>
-      <c r="D100" s="160">
+      <c r="C100" s="123">
+        <v>0</v>
+      </c>
+      <c r="D100" s="125">
         <v>50</v>
       </c>
       <c r="E100" s="57"/>
       <c r="F100" s="58"/>
     </row>
     <row r="101" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="157"/>
-      <c r="B101" s="157"/>
-      <c r="C101" s="159"/>
-      <c r="D101" s="161"/>
+      <c r="A101" s="122"/>
+      <c r="B101" s="122"/>
+      <c r="C101" s="124"/>
+      <c r="D101" s="126"/>
       <c r="E101" s="67" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F101" s="68">
         <v>98</v>
@@ -7723,7 +7726,7 @@
     </row>
     <row r="103" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="B103" s="9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C103" s="1">
         <v>0</v>
@@ -7734,6 +7737,52 @@
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C1:D2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B40:B64"/>
+    <mergeCell ref="C40:C64"/>
+    <mergeCell ref="D40:D64"/>
+    <mergeCell ref="A9:A39"/>
+    <mergeCell ref="B9:B39"/>
+    <mergeCell ref="C9:C39"/>
+    <mergeCell ref="D9:D39"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="A66:A75"/>
+    <mergeCell ref="B66:B75"/>
+    <mergeCell ref="C66:C75"/>
+    <mergeCell ref="D66:D75"/>
+    <mergeCell ref="A79:A81"/>
+    <mergeCell ref="B79:B81"/>
+    <mergeCell ref="C79:C81"/>
+    <mergeCell ref="D79:D81"/>
+    <mergeCell ref="A76:A78"/>
+    <mergeCell ref="B76:B78"/>
+    <mergeCell ref="C76:C78"/>
+    <mergeCell ref="D76:D78"/>
+    <mergeCell ref="A87:A91"/>
+    <mergeCell ref="B87:B91"/>
+    <mergeCell ref="C87:C91"/>
+    <mergeCell ref="D87:D91"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="B82:B86"/>
+    <mergeCell ref="C82:C86"/>
+    <mergeCell ref="D82:D86"/>
+    <mergeCell ref="A100:A101"/>
+    <mergeCell ref="B100:B101"/>
+    <mergeCell ref="C100:C101"/>
+    <mergeCell ref="D100:D101"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="B98:B99"/>
+    <mergeCell ref="C98:C99"/>
+    <mergeCell ref="D98:D99"/>
     <mergeCell ref="E93:F94"/>
     <mergeCell ref="A95:A96"/>
     <mergeCell ref="B95:B96"/>
@@ -7743,52 +7792,6 @@
     <mergeCell ref="B93:B94"/>
     <mergeCell ref="C93:C94"/>
     <mergeCell ref="D93:D94"/>
-    <mergeCell ref="A100:A101"/>
-    <mergeCell ref="B100:B101"/>
-    <mergeCell ref="C100:C101"/>
-    <mergeCell ref="D100:D101"/>
-    <mergeCell ref="A98:A99"/>
-    <mergeCell ref="B98:B99"/>
-    <mergeCell ref="C98:C99"/>
-    <mergeCell ref="D98:D99"/>
-    <mergeCell ref="A87:A91"/>
-    <mergeCell ref="B87:B91"/>
-    <mergeCell ref="C87:C91"/>
-    <mergeCell ref="D87:D91"/>
-    <mergeCell ref="A82:A86"/>
-    <mergeCell ref="B82:B86"/>
-    <mergeCell ref="C82:C86"/>
-    <mergeCell ref="D82:D86"/>
-    <mergeCell ref="A79:A81"/>
-    <mergeCell ref="B79:B81"/>
-    <mergeCell ref="C79:C81"/>
-    <mergeCell ref="D79:D81"/>
-    <mergeCell ref="A76:A78"/>
-    <mergeCell ref="B76:B78"/>
-    <mergeCell ref="C76:C78"/>
-    <mergeCell ref="D76:D78"/>
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="A66:A75"/>
-    <mergeCell ref="B66:B75"/>
-    <mergeCell ref="C66:C75"/>
-    <mergeCell ref="D66:D75"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B40:B64"/>
-    <mergeCell ref="C40:C64"/>
-    <mergeCell ref="D40:D64"/>
-    <mergeCell ref="A9:A39"/>
-    <mergeCell ref="B9:B39"/>
-    <mergeCell ref="C9:C39"/>
-    <mergeCell ref="D9:D39"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C1:D2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7800,8 +7803,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7838,7 +7841,7 @@
         <v>30</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7857,7 +7860,7 @@
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>16</v>
@@ -7881,7 +7884,7 @@
     </row>
     <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>18</v>
@@ -7905,7 +7908,7 @@
     </row>
     <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>19</v>
@@ -7929,7 +7932,7 @@
     </row>
     <row r="6" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>20</v>
@@ -7953,7 +7956,7 @@
     </row>
     <row r="7" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>22</v>
@@ -7977,7 +7980,7 @@
     </row>
     <row r="8" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>23</v>
@@ -8001,7 +8004,7 @@
     </row>
     <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>6</v>
@@ -8085,7 +8088,7 @@
     </row>
     <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>9</v>
@@ -8133,7 +8136,7 @@
     </row>
     <row r="15" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>11</v>
@@ -8184,7 +8187,7 @@
     </row>
     <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="C18" s="9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D18" s="9">
         <v>0</v>
@@ -8200,7 +8203,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -8218,10 +8221,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8247,13 +8250,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -8298,7 +8301,7 @@
     </row>
     <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>118</v>
@@ -8310,7 +8313,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="108"/>
@@ -8412,12 +8415,12 @@
     </row>
     <row r="10" spans="1:8" ht="224" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
       <c r="F10" s="8" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G10" s="108"/>
     </row>
@@ -8429,7 +8432,7 @@
         <v>100</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>70</v>
@@ -8451,7 +8454,7 @@
         <v>83</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E12" s="21" t="s">
         <v>245</v>
@@ -8465,7 +8468,7 @@
     </row>
     <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C14" s="9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D14" s="4">
         <v>0</v>
@@ -8479,21 +8482,17 @@
       <c r="A15" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" s="109" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="109" t="s">
-        <v>466</v>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:8" s="109" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="109" t="s">
+        <v>493</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="G2:G12"/>
-    <mergeCell ref="A17:XFD17"/>
+    <mergeCell ref="A16:XFD16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8505,8 +8504,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8528,10 +8527,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>253</v>
@@ -8539,7 +8538,7 @@
     </row>
     <row r="2" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>121</v>
@@ -8613,7 +8612,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>100</v>
@@ -8703,7 +8702,7 @@
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C12" s="9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D12" s="4">
         <v>0</v>
@@ -8734,10 +8733,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B439655D-7B77-3241-98F2-392F99175C45}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8760,10 +8759,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>468</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>470</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>253</v>
@@ -8791,7 +8790,7 @@
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B3" t="s">
         <v>121</v>
@@ -8866,7 +8865,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D7" s="20" t="s">
         <v>109</v>
@@ -8896,7 +8895,7 @@
     </row>
     <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>125</v>
@@ -8918,7 +8917,7 @@
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C11" s="9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D11" s="4">
         <v>8</v>
@@ -8931,19 +8930,26 @@
       <c r="A12" t="s">
         <v>229</v>
       </c>
+      <c r="D12" s="8"/>
     </row>
     <row r="13" spans="1:6" s="110" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="110" t="s">
         <v>254</v>
       </c>
     </row>
+    <row r="14" spans="1:6" s="109" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="109" t="s">
+        <v>492</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A13:XFD13"/>
     <mergeCell ref="F2:F9"/>
+    <mergeCell ref="A14:XFD14"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A13" r:id="rId1" display="https://jamanetwork.com/journals/jamainternalmedicine/fullarticle/414155" xr:uid="{51103764-FEE0-1B43-B9AE-E2BE2EE789F1}"/>
+    <hyperlink ref="A13" r:id="rId1" display="https://jamanetwork.com/journals/jamainternalmedicine/fullarticle/414155" xr:uid="{E9CFADFE-7C2A-7F40-AE47-B6F06E855F43}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
@@ -8955,7 +8961,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -8980,10 +8986,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="105" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E1" s="105" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="F1" s="104" t="s">
         <v>248</v>
@@ -8995,13 +9001,13 @@
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>251</v>
@@ -9013,13 +9019,13 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>251</v>
@@ -9031,13 +9037,13 @@
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>251</v>
@@ -9045,17 +9051,17 @@
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>251</v>
@@ -9067,13 +9073,13 @@
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8" t="s">
+        <v>477</v>
+      </c>
+      <c r="D6" s="20" t="s">
         <v>479</v>
       </c>
-      <c r="D6" s="20" t="s">
-        <v>481</v>
-      </c>
       <c r="E6" s="20" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>251</v>
@@ -9081,17 +9087,17 @@
     </row>
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>251</v>
@@ -9103,13 +9109,13 @@
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>251</v>
@@ -9117,17 +9123,17 @@
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>251</v>
@@ -9139,13 +9145,13 @@
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>251</v>
@@ -9161,7 +9167,7 @@
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C12" s="9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D12" s="20">
         <v>0</v>
@@ -9177,12 +9183,12 @@
     </row>
     <row r="14" spans="1:6" s="111" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="111" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
   </sheetData>
@@ -9201,10 +9207,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{412F9042-7286-FD43-86C5-30519F0C2582}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9227,10 +9233,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="105" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E1" s="105" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>253</v>
@@ -9258,7 +9264,7 @@
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B3" t="s">
         <v>117</v>
@@ -9276,7 +9282,7 @@
     </row>
     <row r="4" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>96</v>
@@ -9294,7 +9300,7 @@
     </row>
     <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B5" t="s">
         <v>97</v>
@@ -9312,7 +9318,7 @@
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B6" t="s">
         <v>98</v>
@@ -9366,7 +9372,7 @@
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B9" t="s">
         <v>100</v>
@@ -9406,7 +9412,7 @@
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C12" s="9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D12" s="4">
         <v>0</v>
@@ -9419,15 +9425,23 @@
       <c r="A13" t="s">
         <v>229</v>
       </c>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>259</v>
+        <v>258</v>
+      </c>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:6" s="109" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="109" t="s">
+        <v>492</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="F2:F10"/>
+    <mergeCell ref="A15:XFD15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -9439,8 +9453,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9467,10 +9481,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="105" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E1" s="105" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>253</v>
@@ -9478,22 +9492,22 @@
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>269</v>
-      </c>
       <c r="C2" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F2" s="108" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -9504,10 +9518,10 @@
         <v>117</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>94</v>
@@ -9519,13 +9533,13 @@
         <v>17</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E4" s="20" t="s">
         <v>93</v>
@@ -9540,13 +9554,13 @@
         <v>91</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F5" s="108"/>
     </row>
@@ -9558,31 +9572,31 @@
         <v>92</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F6" s="108"/>
     </row>
     <row r="7" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F7" s="108"/>
     </row>
@@ -9594,10 +9608,10 @@
         <v>101</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>244</v>
@@ -9606,37 +9620,37 @@
     </row>
     <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>125</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>244</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F9" s="108"/>
     </row>
     <row r="10" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>249</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>243</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F10" s="108"/>
     </row>
@@ -9648,13 +9662,13 @@
         <v>252</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>244</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F11" s="108"/>
     </row>
@@ -9666,13 +9680,13 @@
         <v>192</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>244</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F12" s="108"/>
     </row>
@@ -9682,7 +9696,7 @@
     </row>
     <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C14" s="9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D14" s="4">
         <v>0</v>
@@ -9698,7 +9712,7 @@
     </row>
     <row r="16" spans="1:6" s="112" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="112" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -9757,22 +9771,22 @@
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>269</v>
-      </c>
       <c r="C2" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D2" s="20">
         <v>0</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F2" s="108" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -9783,7 +9797,7 @@
         <v>117</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D3" s="20">
         <v>0</v>
@@ -9798,10 +9812,10 @@
         <v>17</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D4" s="20">
         <v>0</v>
@@ -9819,13 +9833,13 @@
         <v>91</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D5" s="20">
         <v>0</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F5" s="108"/>
     </row>
@@ -9837,31 +9851,31 @@
         <v>92</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D6" s="20">
         <v>0</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F6" s="108"/>
     </row>
     <row r="7" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D7" s="20">
         <v>0</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F7" s="108"/>
     </row>
@@ -9873,7 +9887,7 @@
         <v>101</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D8" s="20">
         <v>0</v>
@@ -9885,13 +9899,13 @@
     </row>
     <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>125</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>244</v>
@@ -9903,13 +9917,13 @@
     </row>
     <row r="10" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>249</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>243</v>
@@ -9927,7 +9941,7 @@
         <v>252</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>244</v>
@@ -9945,7 +9959,7 @@
         <v>192</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>244</v>
@@ -9962,7 +9976,7 @@
     </row>
     <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C14" s="9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D14" s="4">
         <v>0</v>
@@ -9978,7 +9992,7 @@
     </row>
     <row r="16" spans="1:6" s="112" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="112" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More dietary indexes for NHAENS 1999-2004
HEI2020, AHEI, DASH, DASHI, MED, MEDI available for NHANES 1999-2004
</commit_message>
<xml_diff>
--- a/dietaryindex_SCORING_ALGORITHM.xlsx
+++ b/dietaryindex_SCORING_ALGORITHM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10916"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Desktop/Emory University - Ph.D./dietaryindex_package/dietaryindex publication/Formal_publication/Major revision/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Library/Mobile Documents/com~apple~CloudDocs/Desktop/Emory University - Ph.D./dietaryindex_package/dietaryindex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E84E07A8-75EE-424B-A5EF-D180D4B1310A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9B1BF9-C6BC-3140-B2AA-5E6954FFB5A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11900" yWindow="2840" windowWidth="26000" windowHeight="19420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7980" yWindow="500" windowWidth="25960" windowHeight="19420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HEI2020" sheetId="18" r:id="rId1"/>
@@ -2593,6 +2593,171 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="12" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2604,171 +2769,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="12" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -6486,31 +6486,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="119" t="s">
         <v>310</v>
       </c>
       <c r="B1" s="77" t="s">
         <v>311</v>
       </c>
-      <c r="C1" s="165" t="s">
+      <c r="C1" s="122" t="s">
         <v>312</v>
       </c>
-      <c r="D1" s="166"/>
+      <c r="D1" s="123"/>
       <c r="E1" s="23"/>
       <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6" s="25" customFormat="1" ht="31" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="163"/>
+      <c r="A2" s="120"/>
       <c r="B2" s="78" t="s">
         <v>313</v>
       </c>
-      <c r="C2" s="167"/>
-      <c r="D2" s="168"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="125"/>
       <c r="E2" s="23"/>
       <c r="F2" s="24"/>
     </row>
     <row r="3" spans="1:6" s="29" customFormat="1" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="164"/>
+      <c r="A3" s="121"/>
       <c r="B3" s="26" t="s">
         <v>314</v>
       </c>
@@ -6528,13 +6528,13 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="169" t="s">
+      <c r="A4" s="126" t="s">
         <v>319</v>
       </c>
-      <c r="B4" s="170" t="s">
+      <c r="B4" s="128" t="s">
         <v>320</v>
       </c>
-      <c r="C4" s="137">
+      <c r="C4" s="130">
         <v>0</v>
       </c>
       <c r="D4" s="30" t="s">
@@ -6546,9 +6546,9 @@
       <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="161"/>
-      <c r="B5" s="171"/>
-      <c r="C5" s="160"/>
+      <c r="A5" s="127"/>
+      <c r="B5" s="129"/>
+      <c r="C5" s="131"/>
       <c r="D5" s="33" t="s">
         <v>323</v>
       </c>
@@ -6556,16 +6556,16 @@
       <c r="F5" s="32"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="117" t="s">
+      <c r="A6" s="113" t="s">
         <v>324</v>
       </c>
-      <c r="B6" s="119" t="s">
+      <c r="B6" s="115" t="s">
         <v>325</v>
       </c>
-      <c r="C6" s="117" t="s">
+      <c r="C6" s="113" t="s">
         <v>326</v>
       </c>
-      <c r="D6" s="157" t="s">
+      <c r="D6" s="117" t="s">
         <v>327</v>
       </c>
       <c r="E6" s="92" t="s">
@@ -6576,10 +6576,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="144"/>
-      <c r="B7" s="145"/>
-      <c r="C7" s="144"/>
-      <c r="D7" s="158"/>
+      <c r="A7" s="114"/>
+      <c r="B7" s="116"/>
+      <c r="C7" s="114"/>
+      <c r="D7" s="118"/>
       <c r="E7" s="94" t="s">
         <v>329</v>
       </c>
@@ -6588,10 +6588,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="144"/>
-      <c r="B8" s="145"/>
-      <c r="C8" s="144"/>
-      <c r="D8" s="158"/>
+      <c r="A8" s="114"/>
+      <c r="B8" s="116"/>
+      <c r="C8" s="114"/>
+      <c r="D8" s="118"/>
       <c r="E8" s="94" t="s">
         <v>330</v>
       </c>
@@ -6600,16 +6600,16 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="135" t="s">
+      <c r="A9" s="132" t="s">
         <v>331</v>
       </c>
-      <c r="B9" s="137" t="s">
+      <c r="B9" s="130" t="s">
         <v>332</v>
       </c>
-      <c r="C9" s="137">
-        <v>0</v>
-      </c>
-      <c r="D9" s="137" t="s">
+      <c r="C9" s="130">
+        <v>0</v>
+      </c>
+      <c r="D9" s="130" t="s">
         <v>333</v>
       </c>
       <c r="E9" s="34" t="s">
@@ -6620,10 +6620,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="136"/>
-      <c r="B10" s="138"/>
-      <c r="C10" s="138"/>
-      <c r="D10" s="138"/>
+      <c r="A10" s="133"/>
+      <c r="B10" s="134"/>
+      <c r="C10" s="134"/>
+      <c r="D10" s="134"/>
       <c r="E10" s="36" t="s">
         <v>335</v>
       </c>
@@ -6632,10 +6632,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="136"/>
-      <c r="B11" s="138"/>
-      <c r="C11" s="138"/>
-      <c r="D11" s="138"/>
+      <c r="A11" s="133"/>
+      <c r="B11" s="134"/>
+      <c r="C11" s="134"/>
+      <c r="D11" s="134"/>
       <c r="E11" s="36" t="s">
         <v>336</v>
       </c>
@@ -6644,18 +6644,18 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="136"/>
-      <c r="B12" s="138"/>
-      <c r="C12" s="138"/>
-      <c r="D12" s="138"/>
+      <c r="A12" s="133"/>
+      <c r="B12" s="134"/>
+      <c r="C12" s="134"/>
+      <c r="D12" s="134"/>
       <c r="E12" s="36"/>
       <c r="F12" s="37"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="136"/>
-      <c r="B13" s="138"/>
-      <c r="C13" s="138"/>
-      <c r="D13" s="138"/>
+      <c r="A13" s="133"/>
+      <c r="B13" s="134"/>
+      <c r="C13" s="134"/>
+      <c r="D13" s="134"/>
       <c r="E13" s="36" t="s">
         <v>337</v>
       </c>
@@ -6664,10 +6664,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="136"/>
-      <c r="B14" s="138"/>
-      <c r="C14" s="138"/>
-      <c r="D14" s="138"/>
+      <c r="A14" s="133"/>
+      <c r="B14" s="134"/>
+      <c r="C14" s="134"/>
+      <c r="D14" s="134"/>
       <c r="E14" s="36" t="s">
         <v>338</v>
       </c>
@@ -6676,10 +6676,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="136"/>
-      <c r="B15" s="138"/>
-      <c r="C15" s="138"/>
-      <c r="D15" s="138"/>
+      <c r="A15" s="133"/>
+      <c r="B15" s="134"/>
+      <c r="C15" s="134"/>
+      <c r="D15" s="134"/>
       <c r="E15" s="36" t="s">
         <v>339</v>
       </c>
@@ -6688,10 +6688,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="136"/>
-      <c r="B16" s="138"/>
-      <c r="C16" s="138"/>
-      <c r="D16" s="138"/>
+      <c r="A16" s="133"/>
+      <c r="B16" s="134"/>
+      <c r="C16" s="134"/>
+      <c r="D16" s="134"/>
       <c r="E16" s="36" t="s">
         <v>340</v>
       </c>
@@ -6700,10 +6700,10 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="136"/>
-      <c r="B17" s="138"/>
-      <c r="C17" s="138"/>
-      <c r="D17" s="138"/>
+      <c r="A17" s="133"/>
+      <c r="B17" s="134"/>
+      <c r="C17" s="134"/>
+      <c r="D17" s="134"/>
       <c r="E17" s="36" t="s">
         <v>341</v>
       </c>
@@ -6712,10 +6712,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="136"/>
-      <c r="B18" s="138"/>
-      <c r="C18" s="138"/>
-      <c r="D18" s="138"/>
+      <c r="A18" s="133"/>
+      <c r="B18" s="134"/>
+      <c r="C18" s="134"/>
+      <c r="D18" s="134"/>
       <c r="E18" s="36" t="s">
         <v>342</v>
       </c>
@@ -6724,10 +6724,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="136"/>
-      <c r="B19" s="138"/>
-      <c r="C19" s="138"/>
-      <c r="D19" s="138"/>
+      <c r="A19" s="133"/>
+      <c r="B19" s="134"/>
+      <c r="C19" s="134"/>
+      <c r="D19" s="134"/>
       <c r="E19" s="36" t="s">
         <v>343</v>
       </c>
@@ -6736,10 +6736,10 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="136"/>
-      <c r="B20" s="138"/>
-      <c r="C20" s="138"/>
-      <c r="D20" s="138"/>
+      <c r="A20" s="133"/>
+      <c r="B20" s="134"/>
+      <c r="C20" s="134"/>
+      <c r="D20" s="134"/>
       <c r="E20" s="36" t="s">
         <v>344</v>
       </c>
@@ -6748,10 +6748,10 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="136"/>
-      <c r="B21" s="138"/>
-      <c r="C21" s="138"/>
-      <c r="D21" s="138"/>
+      <c r="A21" s="133"/>
+      <c r="B21" s="134"/>
+      <c r="C21" s="134"/>
+      <c r="D21" s="134"/>
       <c r="E21" s="36" t="s">
         <v>345</v>
       </c>
@@ -6760,10 +6760,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="136"/>
-      <c r="B22" s="138"/>
-      <c r="C22" s="138"/>
-      <c r="D22" s="138"/>
+      <c r="A22" s="133"/>
+      <c r="B22" s="134"/>
+      <c r="C22" s="134"/>
+      <c r="D22" s="134"/>
       <c r="E22" s="36" t="s">
         <v>346</v>
       </c>
@@ -6772,10 +6772,10 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="136"/>
-      <c r="B23" s="138"/>
-      <c r="C23" s="138"/>
-      <c r="D23" s="138"/>
+      <c r="A23" s="133"/>
+      <c r="B23" s="134"/>
+      <c r="C23" s="134"/>
+      <c r="D23" s="134"/>
       <c r="E23" s="36" t="s">
         <v>347</v>
       </c>
@@ -6784,10 +6784,10 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="136"/>
-      <c r="B24" s="138"/>
-      <c r="C24" s="138"/>
-      <c r="D24" s="138"/>
+      <c r="A24" s="133"/>
+      <c r="B24" s="134"/>
+      <c r="C24" s="134"/>
+      <c r="D24" s="134"/>
       <c r="E24" s="36" t="s">
         <v>348</v>
       </c>
@@ -6796,10 +6796,10 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="136"/>
-      <c r="B25" s="138"/>
-      <c r="C25" s="138"/>
-      <c r="D25" s="138"/>
+      <c r="A25" s="133"/>
+      <c r="B25" s="134"/>
+      <c r="C25" s="134"/>
+      <c r="D25" s="134"/>
       <c r="E25" s="36" t="s">
         <v>349</v>
       </c>
@@ -6808,10 +6808,10 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="136"/>
-      <c r="B26" s="138"/>
-      <c r="C26" s="138"/>
-      <c r="D26" s="138"/>
+      <c r="A26" s="133"/>
+      <c r="B26" s="134"/>
+      <c r="C26" s="134"/>
+      <c r="D26" s="134"/>
       <c r="E26" s="36" t="s">
         <v>350</v>
       </c>
@@ -6820,10 +6820,10 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="136"/>
-      <c r="B27" s="138"/>
-      <c r="C27" s="138"/>
-      <c r="D27" s="138"/>
+      <c r="A27" s="133"/>
+      <c r="B27" s="134"/>
+      <c r="C27" s="134"/>
+      <c r="D27" s="134"/>
       <c r="E27" s="36" t="s">
         <v>351</v>
       </c>
@@ -6832,10 +6832,10 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="136"/>
-      <c r="B28" s="138"/>
-      <c r="C28" s="138"/>
-      <c r="D28" s="138"/>
+      <c r="A28" s="133"/>
+      <c r="B28" s="134"/>
+      <c r="C28" s="134"/>
+      <c r="D28" s="134"/>
       <c r="E28" s="36" t="s">
         <v>352</v>
       </c>
@@ -6844,10 +6844,10 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="136"/>
-      <c r="B29" s="138"/>
-      <c r="C29" s="138"/>
-      <c r="D29" s="138"/>
+      <c r="A29" s="133"/>
+      <c r="B29" s="134"/>
+      <c r="C29" s="134"/>
+      <c r="D29" s="134"/>
       <c r="E29" s="36" t="s">
         <v>353</v>
       </c>
@@ -6856,10 +6856,10 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="136"/>
-      <c r="B30" s="138"/>
-      <c r="C30" s="138"/>
-      <c r="D30" s="138"/>
+      <c r="A30" s="133"/>
+      <c r="B30" s="134"/>
+      <c r="C30" s="134"/>
+      <c r="D30" s="134"/>
       <c r="E30" s="36" t="s">
         <v>354</v>
       </c>
@@ -6868,10 +6868,10 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="136"/>
-      <c r="B31" s="138"/>
-      <c r="C31" s="138"/>
-      <c r="D31" s="138"/>
+      <c r="A31" s="133"/>
+      <c r="B31" s="134"/>
+      <c r="C31" s="134"/>
+      <c r="D31" s="134"/>
       <c r="E31" s="36" t="s">
         <v>355</v>
       </c>
@@ -6880,10 +6880,10 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="136"/>
-      <c r="B32" s="138"/>
-      <c r="C32" s="138"/>
-      <c r="D32" s="138"/>
+      <c r="A32" s="133"/>
+      <c r="B32" s="134"/>
+      <c r="C32" s="134"/>
+      <c r="D32" s="134"/>
       <c r="E32" s="36" t="s">
         <v>356</v>
       </c>
@@ -6892,10 +6892,10 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="136"/>
-      <c r="B33" s="138"/>
-      <c r="C33" s="138"/>
-      <c r="D33" s="138"/>
+      <c r="A33" s="133"/>
+      <c r="B33" s="134"/>
+      <c r="C33" s="134"/>
+      <c r="D33" s="134"/>
       <c r="E33" s="36" t="s">
         <v>357</v>
       </c>
@@ -6904,20 +6904,20 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="136"/>
-      <c r="B34" s="138"/>
-      <c r="C34" s="138"/>
-      <c r="D34" s="138"/>
+      <c r="A34" s="133"/>
+      <c r="B34" s="134"/>
+      <c r="C34" s="134"/>
+      <c r="D34" s="134"/>
       <c r="E34" s="36"/>
       <c r="F34" s="38"/>
       <c r="G34" s="8"/>
       <c r="H34" s="39"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="136"/>
-      <c r="B35" s="138"/>
-      <c r="C35" s="138"/>
-      <c r="D35" s="138"/>
+      <c r="A35" s="133"/>
+      <c r="B35" s="134"/>
+      <c r="C35" s="134"/>
+      <c r="D35" s="134"/>
       <c r="E35" s="36" t="s">
         <v>358</v>
       </c>
@@ -6926,18 +6926,18 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="136"/>
-      <c r="B36" s="138"/>
-      <c r="C36" s="138"/>
-      <c r="D36" s="138"/>
+      <c r="A36" s="133"/>
+      <c r="B36" s="134"/>
+      <c r="C36" s="134"/>
+      <c r="D36" s="134"/>
       <c r="E36" s="36"/>
       <c r="F36" s="38"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="136"/>
-      <c r="B37" s="138"/>
-      <c r="C37" s="138"/>
-      <c r="D37" s="138"/>
+      <c r="A37" s="133"/>
+      <c r="B37" s="134"/>
+      <c r="C37" s="134"/>
+      <c r="D37" s="134"/>
       <c r="E37" s="36" t="s">
         <v>359</v>
       </c>
@@ -6946,10 +6946,10 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="136"/>
-      <c r="B38" s="138"/>
-      <c r="C38" s="138"/>
-      <c r="D38" s="138"/>
+      <c r="A38" s="133"/>
+      <c r="B38" s="134"/>
+      <c r="C38" s="134"/>
+      <c r="D38" s="134"/>
       <c r="E38" s="36" t="s">
         <v>360</v>
       </c>
@@ -6958,10 +6958,10 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="161"/>
-      <c r="B39" s="160"/>
-      <c r="C39" s="160"/>
-      <c r="D39" s="160"/>
+      <c r="A39" s="127"/>
+      <c r="B39" s="131"/>
+      <c r="C39" s="131"/>
+      <c r="D39" s="131"/>
       <c r="E39" s="40" t="s">
         <v>361</v>
       </c>
@@ -6970,16 +6970,16 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="135" t="s">
+      <c r="A40" s="132" t="s">
         <v>362</v>
       </c>
-      <c r="B40" s="137" t="s">
+      <c r="B40" s="130" t="s">
         <v>363</v>
       </c>
-      <c r="C40" s="137">
-        <v>0</v>
-      </c>
-      <c r="D40" s="137" t="s">
+      <c r="C40" s="130">
+        <v>0</v>
+      </c>
+      <c r="D40" s="130" t="s">
         <v>364</v>
       </c>
       <c r="E40" s="42" t="s">
@@ -6990,18 +6990,18 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="136"/>
-      <c r="B41" s="138"/>
-      <c r="C41" s="138"/>
-      <c r="D41" s="138"/>
+      <c r="A41" s="133"/>
+      <c r="B41" s="134"/>
+      <c r="C41" s="134"/>
+      <c r="D41" s="134"/>
       <c r="E41" s="44"/>
       <c r="F41" s="45"/>
     </row>
     <row r="42" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="136"/>
-      <c r="B42" s="138"/>
-      <c r="C42" s="138"/>
-      <c r="D42" s="138"/>
+      <c r="A42" s="133"/>
+      <c r="B42" s="134"/>
+      <c r="C42" s="134"/>
+      <c r="D42" s="134"/>
       <c r="E42" s="44" t="s">
         <v>366</v>
       </c>
@@ -7010,10 +7010,10 @@
       </c>
     </row>
     <row r="43" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="136"/>
-      <c r="B43" s="138"/>
-      <c r="C43" s="138"/>
-      <c r="D43" s="138"/>
+      <c r="A43" s="133"/>
+      <c r="B43" s="134"/>
+      <c r="C43" s="134"/>
+      <c r="D43" s="134"/>
       <c r="E43" s="44" t="s">
         <v>367</v>
       </c>
@@ -7023,9 +7023,9 @@
     </row>
     <row r="44" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="30"/>
-      <c r="B44" s="138"/>
-      <c r="C44" s="138"/>
-      <c r="D44" s="138"/>
+      <c r="B44" s="134"/>
+      <c r="C44" s="134"/>
+      <c r="D44" s="134"/>
       <c r="E44" s="44" t="s">
         <v>368</v>
       </c>
@@ -7035,9 +7035,9 @@
     </row>
     <row r="45" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="30"/>
-      <c r="B45" s="138"/>
-      <c r="C45" s="138"/>
-      <c r="D45" s="138"/>
+      <c r="B45" s="134"/>
+      <c r="C45" s="134"/>
+      <c r="D45" s="134"/>
       <c r="E45" s="44" t="s">
         <v>369</v>
       </c>
@@ -7047,9 +7047,9 @@
     </row>
     <row r="46" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="30"/>
-      <c r="B46" s="138"/>
-      <c r="C46" s="138"/>
-      <c r="D46" s="138"/>
+      <c r="B46" s="134"/>
+      <c r="C46" s="134"/>
+      <c r="D46" s="134"/>
       <c r="E46" s="44" t="s">
         <v>370</v>
       </c>
@@ -7059,9 +7059,9 @@
     </row>
     <row r="47" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="30"/>
-      <c r="B47" s="138"/>
-      <c r="C47" s="138"/>
-      <c r="D47" s="138"/>
+      <c r="B47" s="134"/>
+      <c r="C47" s="134"/>
+      <c r="D47" s="134"/>
       <c r="E47" s="44" t="s">
         <v>371</v>
       </c>
@@ -7071,9 +7071,9 @@
     </row>
     <row r="48" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="30"/>
-      <c r="B48" s="138"/>
-      <c r="C48" s="138"/>
-      <c r="D48" s="138"/>
+      <c r="B48" s="134"/>
+      <c r="C48" s="134"/>
+      <c r="D48" s="134"/>
       <c r="E48" s="44" t="s">
         <v>372</v>
       </c>
@@ -7083,17 +7083,17 @@
     </row>
     <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="30"/>
-      <c r="B49" s="138"/>
-      <c r="C49" s="138"/>
-      <c r="D49" s="138"/>
+      <c r="B49" s="134"/>
+      <c r="C49" s="134"/>
+      <c r="D49" s="134"/>
       <c r="E49" s="44"/>
       <c r="F49" s="45"/>
     </row>
     <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="30"/>
-      <c r="B50" s="138"/>
-      <c r="C50" s="138"/>
-      <c r="D50" s="138"/>
+      <c r="B50" s="134"/>
+      <c r="C50" s="134"/>
+      <c r="D50" s="134"/>
       <c r="E50" s="44" t="s">
         <v>373</v>
       </c>
@@ -7103,9 +7103,9 @@
     </row>
     <row r="51" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="30"/>
-      <c r="B51" s="138"/>
-      <c r="C51" s="138"/>
-      <c r="D51" s="138"/>
+      <c r="B51" s="134"/>
+      <c r="C51" s="134"/>
+      <c r="D51" s="134"/>
       <c r="E51" s="44" t="s">
         <v>374</v>
       </c>
@@ -7115,9 +7115,9 @@
     </row>
     <row r="52" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="30"/>
-      <c r="B52" s="138"/>
-      <c r="C52" s="138"/>
-      <c r="D52" s="138"/>
+      <c r="B52" s="134"/>
+      <c r="C52" s="134"/>
+      <c r="D52" s="134"/>
       <c r="E52" s="44" t="s">
         <v>375</v>
       </c>
@@ -7127,9 +7127,9 @@
     </row>
     <row r="53" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="30"/>
-      <c r="B53" s="138"/>
-      <c r="C53" s="138"/>
-      <c r="D53" s="138"/>
+      <c r="B53" s="134"/>
+      <c r="C53" s="134"/>
+      <c r="D53" s="134"/>
       <c r="E53" s="44" t="s">
         <v>376</v>
       </c>
@@ -7139,9 +7139,9 @@
     </row>
     <row r="54" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="30"/>
-      <c r="B54" s="138"/>
-      <c r="C54" s="138"/>
-      <c r="D54" s="138"/>
+      <c r="B54" s="134"/>
+      <c r="C54" s="134"/>
+      <c r="D54" s="134"/>
       <c r="E54" s="44" t="s">
         <v>377</v>
       </c>
@@ -7151,17 +7151,17 @@
     </row>
     <row r="55" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="30"/>
-      <c r="B55" s="138"/>
-      <c r="C55" s="138"/>
-      <c r="D55" s="138"/>
+      <c r="B55" s="134"/>
+      <c r="C55" s="134"/>
+      <c r="D55" s="134"/>
       <c r="E55" s="44"/>
       <c r="F55" s="37"/>
     </row>
     <row r="56" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="30"/>
-      <c r="B56" s="138"/>
-      <c r="C56" s="138"/>
-      <c r="D56" s="138"/>
+      <c r="B56" s="134"/>
+      <c r="C56" s="134"/>
+      <c r="D56" s="134"/>
       <c r="E56" s="44" t="s">
         <v>378</v>
       </c>
@@ -7171,25 +7171,25 @@
     </row>
     <row r="57" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="30"/>
-      <c r="B57" s="138"/>
-      <c r="C57" s="138"/>
-      <c r="D57" s="138"/>
+      <c r="B57" s="134"/>
+      <c r="C57" s="134"/>
+      <c r="D57" s="134"/>
       <c r="E57" s="44"/>
       <c r="F57" s="45"/>
     </row>
     <row r="58" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="30"/>
-      <c r="B58" s="138"/>
-      <c r="C58" s="138"/>
-      <c r="D58" s="138"/>
+      <c r="B58" s="134"/>
+      <c r="C58" s="134"/>
+      <c r="D58" s="134"/>
       <c r="E58" s="44"/>
       <c r="F58" s="45"/>
     </row>
     <row r="59" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="30"/>
-      <c r="B59" s="138"/>
-      <c r="C59" s="138"/>
-      <c r="D59" s="138"/>
+      <c r="B59" s="134"/>
+      <c r="C59" s="134"/>
+      <c r="D59" s="134"/>
       <c r="E59" s="44" t="s">
         <v>379</v>
       </c>
@@ -7199,9 +7199,9 @@
     </row>
     <row r="60" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="30"/>
-      <c r="B60" s="138"/>
-      <c r="C60" s="138"/>
-      <c r="D60" s="138"/>
+      <c r="B60" s="134"/>
+      <c r="C60" s="134"/>
+      <c r="D60" s="134"/>
       <c r="E60" s="44" t="s">
         <v>380</v>
       </c>
@@ -7211,9 +7211,9 @@
     </row>
     <row r="61" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="30"/>
-      <c r="B61" s="138"/>
-      <c r="C61" s="138"/>
-      <c r="D61" s="138"/>
+      <c r="B61" s="134"/>
+      <c r="C61" s="134"/>
+      <c r="D61" s="134"/>
       <c r="E61" s="44" t="s">
         <v>381</v>
       </c>
@@ -7223,25 +7223,25 @@
     </row>
     <row r="62" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="30"/>
-      <c r="B62" s="138"/>
-      <c r="C62" s="138"/>
-      <c r="D62" s="138"/>
+      <c r="B62" s="134"/>
+      <c r="C62" s="134"/>
+      <c r="D62" s="134"/>
       <c r="E62" s="44"/>
       <c r="F62" s="45"/>
     </row>
     <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="30"/>
-      <c r="B63" s="138"/>
-      <c r="C63" s="138"/>
-      <c r="D63" s="138"/>
+      <c r="B63" s="134"/>
+      <c r="C63" s="134"/>
+      <c r="D63" s="134"/>
       <c r="E63" s="44"/>
       <c r="F63" s="45"/>
     </row>
     <row r="64" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="30"/>
-      <c r="B64" s="160"/>
-      <c r="C64" s="160"/>
-      <c r="D64" s="160"/>
+      <c r="B64" s="131"/>
+      <c r="C64" s="131"/>
+      <c r="D64" s="131"/>
       <c r="E64" s="46"/>
       <c r="F64" s="47"/>
     </row>
@@ -7258,22 +7258,22 @@
       <c r="D65" s="91" t="s">
         <v>385</v>
       </c>
-      <c r="E65" s="152" t="s">
+      <c r="E65" s="135" t="s">
         <v>386</v>
       </c>
-      <c r="F65" s="153"/>
+      <c r="F65" s="136"/>
     </row>
     <row r="66" spans="1:6" ht="29.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="117" t="s">
+      <c r="A66" s="113" t="s">
         <v>387</v>
       </c>
-      <c r="B66" s="119" t="s">
+      <c r="B66" s="115" t="s">
         <v>388</v>
       </c>
-      <c r="C66" s="154" t="s">
+      <c r="C66" s="139" t="s">
         <v>389</v>
       </c>
-      <c r="D66" s="157" t="s">
+      <c r="D66" s="117" t="s">
         <v>390</v>
       </c>
       <c r="E66" s="49" t="s">
@@ -7284,18 +7284,18 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" s="144"/>
-      <c r="B67" s="145"/>
-      <c r="C67" s="155"/>
-      <c r="D67" s="158"/>
+      <c r="A67" s="114"/>
+      <c r="B67" s="116"/>
+      <c r="C67" s="140"/>
+      <c r="D67" s="118"/>
       <c r="E67" s="51"/>
       <c r="F67" s="52"/>
     </row>
     <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A68" s="144"/>
-      <c r="B68" s="145"/>
-      <c r="C68" s="155"/>
-      <c r="D68" s="158"/>
+      <c r="A68" s="114"/>
+      <c r="B68" s="116"/>
+      <c r="C68" s="140"/>
+      <c r="D68" s="118"/>
       <c r="E68" s="51" t="s">
         <v>392</v>
       </c>
@@ -7304,18 +7304,18 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A69" s="144"/>
-      <c r="B69" s="145"/>
-      <c r="C69" s="155"/>
-      <c r="D69" s="158"/>
+      <c r="A69" s="114"/>
+      <c r="B69" s="116"/>
+      <c r="C69" s="140"/>
+      <c r="D69" s="118"/>
       <c r="E69" s="51"/>
       <c r="F69" s="52"/>
     </row>
     <row r="70" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A70" s="144"/>
-      <c r="B70" s="145"/>
-      <c r="C70" s="155"/>
-      <c r="D70" s="158"/>
+      <c r="A70" s="114"/>
+      <c r="B70" s="116"/>
+      <c r="C70" s="140"/>
+      <c r="D70" s="118"/>
       <c r="E70" s="51" t="s">
         <v>393</v>
       </c>
@@ -7324,10 +7324,10 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A71" s="144"/>
-      <c r="B71" s="145"/>
-      <c r="C71" s="155"/>
-      <c r="D71" s="158"/>
+      <c r="A71" s="114"/>
+      <c r="B71" s="116"/>
+      <c r="C71" s="140"/>
+      <c r="D71" s="118"/>
       <c r="E71" s="51" t="s">
         <v>394</v>
       </c>
@@ -7336,18 +7336,18 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A72" s="144"/>
-      <c r="B72" s="145"/>
-      <c r="C72" s="155"/>
-      <c r="D72" s="158"/>
+      <c r="A72" s="114"/>
+      <c r="B72" s="116"/>
+      <c r="C72" s="140"/>
+      <c r="D72" s="118"/>
       <c r="E72" s="51"/>
       <c r="F72" s="52"/>
     </row>
     <row r="73" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A73" s="144"/>
-      <c r="B73" s="145"/>
-      <c r="C73" s="155"/>
-      <c r="D73" s="158"/>
+      <c r="A73" s="114"/>
+      <c r="B73" s="116"/>
+      <c r="C73" s="140"/>
+      <c r="D73" s="118"/>
       <c r="E73" s="51" t="s">
         <v>395</v>
       </c>
@@ -7356,18 +7356,18 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A74" s="144"/>
-      <c r="B74" s="145"/>
-      <c r="C74" s="155"/>
-      <c r="D74" s="158"/>
+      <c r="A74" s="114"/>
+      <c r="B74" s="116"/>
+      <c r="C74" s="140"/>
+      <c r="D74" s="118"/>
       <c r="E74" s="51"/>
       <c r="F74" s="52"/>
     </row>
     <row r="75" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="118"/>
-      <c r="B75" s="120"/>
-      <c r="C75" s="156"/>
-      <c r="D75" s="159"/>
+      <c r="A75" s="137"/>
+      <c r="B75" s="138"/>
+      <c r="C75" s="141"/>
+      <c r="D75" s="142"/>
       <c r="E75" s="53" t="s">
         <v>396</v>
       </c>
@@ -7376,26 +7376,26 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="29.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="117" t="s">
+      <c r="A76" s="113" t="s">
         <v>397</v>
       </c>
-      <c r="B76" s="119" t="s">
+      <c r="B76" s="115" t="s">
         <v>398</v>
       </c>
-      <c r="C76" s="149" t="s">
+      <c r="C76" s="146" t="s">
         <v>389</v>
       </c>
-      <c r="D76" s="146" t="s">
+      <c r="D76" s="143" t="s">
         <v>399</v>
       </c>
       <c r="E76" s="81"/>
       <c r="F76" s="82"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="144"/>
-      <c r="B77" s="145"/>
-      <c r="C77" s="150"/>
-      <c r="D77" s="147"/>
+      <c r="A77" s="114"/>
+      <c r="B77" s="116"/>
+      <c r="C77" s="147"/>
+      <c r="D77" s="144"/>
       <c r="E77" s="83" t="s">
         <v>400</v>
       </c>
@@ -7404,10 +7404,10 @@
       </c>
     </row>
     <row r="78" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="118"/>
-      <c r="B78" s="120"/>
-      <c r="C78" s="151"/>
-      <c r="D78" s="148"/>
+      <c r="A78" s="137"/>
+      <c r="B78" s="138"/>
+      <c r="C78" s="148"/>
+      <c r="D78" s="145"/>
       <c r="E78" s="85" t="s">
         <v>401</v>
       </c>
@@ -7416,16 +7416,16 @@
       </c>
     </row>
     <row r="79" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="117" t="s">
+      <c r="A79" s="113" t="s">
         <v>402</v>
       </c>
-      <c r="B79" s="119" t="s">
+      <c r="B79" s="115" t="s">
         <v>403</v>
       </c>
-      <c r="C79" s="119" t="s">
+      <c r="C79" s="115" t="s">
         <v>404</v>
       </c>
-      <c r="D79" s="146" t="s">
+      <c r="D79" s="143" t="s">
         <v>405</v>
       </c>
       <c r="E79" s="87" t="s">
@@ -7436,32 +7436,32 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="144"/>
-      <c r="B80" s="145"/>
-      <c r="C80" s="145"/>
-      <c r="D80" s="147"/>
+      <c r="A80" s="114"/>
+      <c r="B80" s="116"/>
+      <c r="C80" s="116"/>
+      <c r="D80" s="144"/>
       <c r="E80" s="83"/>
       <c r="F80" s="89"/>
     </row>
     <row r="81" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="118"/>
-      <c r="B81" s="120"/>
-      <c r="C81" s="120"/>
-      <c r="D81" s="148"/>
+      <c r="A81" s="137"/>
+      <c r="B81" s="138"/>
+      <c r="C81" s="138"/>
+      <c r="D81" s="145"/>
       <c r="E81" s="85"/>
       <c r="F81" s="90"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A82" s="127" t="s">
+      <c r="A82" s="149" t="s">
         <v>407</v>
       </c>
-      <c r="B82" s="131" t="s">
+      <c r="B82" s="151" t="s">
         <v>408</v>
       </c>
-      <c r="C82" s="141">
-        <v>0</v>
-      </c>
-      <c r="D82" s="141" t="s">
+      <c r="C82" s="153">
+        <v>0</v>
+      </c>
+      <c r="D82" s="153" t="s">
         <v>409</v>
       </c>
       <c r="E82" s="96" t="s">
@@ -7472,19 +7472,19 @@
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A83" s="139"/>
-      <c r="B83" s="140"/>
-      <c r="C83" s="142"/>
-      <c r="D83" s="142"/>
+      <c r="A83" s="150"/>
+      <c r="B83" s="152"/>
+      <c r="C83" s="154"/>
+      <c r="D83" s="154"/>
       <c r="E83" s="98"/>
       <c r="F83" s="99"/>
       <c r="G83" s="55"/>
     </row>
     <row r="84" spans="1:7" s="56" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="139"/>
-      <c r="B84" s="140"/>
-      <c r="C84" s="142"/>
-      <c r="D84" s="142"/>
+      <c r="A84" s="150"/>
+      <c r="B84" s="152"/>
+      <c r="C84" s="154"/>
+      <c r="D84" s="154"/>
       <c r="E84" s="98" t="s">
         <v>411</v>
       </c>
@@ -7493,10 +7493,10 @@
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A85" s="139"/>
-      <c r="B85" s="140"/>
-      <c r="C85" s="142"/>
-      <c r="D85" s="142"/>
+      <c r="A85" s="150"/>
+      <c r="B85" s="152"/>
+      <c r="C85" s="154"/>
+      <c r="D85" s="154"/>
       <c r="E85" s="98" t="s">
         <v>412</v>
       </c>
@@ -7505,10 +7505,10 @@
       </c>
     </row>
     <row r="86" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="139"/>
-      <c r="B86" s="140"/>
-      <c r="C86" s="142"/>
-      <c r="D86" s="143"/>
+      <c r="A86" s="150"/>
+      <c r="B86" s="152"/>
+      <c r="C86" s="154"/>
+      <c r="D86" s="155"/>
       <c r="E86" s="100" t="s">
         <v>413</v>
       </c>
@@ -7517,16 +7517,16 @@
       </c>
     </row>
     <row r="87" spans="1:7" ht="43.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="135" t="s">
+      <c r="A87" s="132" t="s">
         <v>414</v>
       </c>
-      <c r="B87" s="135" t="s">
+      <c r="B87" s="132" t="s">
         <v>415</v>
       </c>
-      <c r="C87" s="137">
-        <v>0</v>
-      </c>
-      <c r="D87" s="137" t="s">
+      <c r="C87" s="130">
+        <v>0</v>
+      </c>
+      <c r="D87" s="130" t="s">
         <v>416</v>
       </c>
       <c r="E87" s="57" t="s">
@@ -7537,10 +7537,10 @@
       </c>
     </row>
     <row r="88" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A88" s="136"/>
-      <c r="B88" s="136"/>
-      <c r="C88" s="138"/>
-      <c r="D88" s="138"/>
+      <c r="A88" s="133"/>
+      <c r="B88" s="133"/>
+      <c r="C88" s="134"/>
+      <c r="D88" s="134"/>
       <c r="E88" s="59" t="s">
         <v>418</v>
       </c>
@@ -7549,18 +7549,18 @@
       </c>
     </row>
     <row r="89" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A89" s="136"/>
-      <c r="B89" s="136"/>
-      <c r="C89" s="138"/>
-      <c r="D89" s="138"/>
+      <c r="A89" s="133"/>
+      <c r="B89" s="133"/>
+      <c r="C89" s="134"/>
+      <c r="D89" s="134"/>
       <c r="E89" s="59"/>
       <c r="F89" s="60"/>
     </row>
     <row r="90" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A90" s="136"/>
-      <c r="B90" s="136"/>
-      <c r="C90" s="138"/>
-      <c r="D90" s="138"/>
+      <c r="A90" s="133"/>
+      <c r="B90" s="133"/>
+      <c r="C90" s="134"/>
+      <c r="D90" s="134"/>
       <c r="E90" s="61" t="s">
         <v>419</v>
       </c>
@@ -7569,10 +7569,10 @@
       </c>
     </row>
     <row r="91" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="136"/>
-      <c r="B91" s="136"/>
-      <c r="C91" s="138"/>
-      <c r="D91" s="138"/>
+      <c r="A91" s="133"/>
+      <c r="B91" s="133"/>
+      <c r="C91" s="134"/>
+      <c r="D91" s="134"/>
       <c r="E91" s="61"/>
       <c r="F91" s="62"/>
     </row>
@@ -7595,42 +7595,42 @@
       <c r="F92" s="71"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A93" s="117" t="s">
+      <c r="A93" s="113" t="s">
         <v>430</v>
       </c>
-      <c r="B93" s="119" t="s">
+      <c r="B93" s="115" t="s">
         <v>431</v>
       </c>
-      <c r="C93" s="119" t="s">
+      <c r="C93" s="115" t="s">
         <v>432</v>
       </c>
-      <c r="D93" s="119" t="s">
+      <c r="D93" s="115" t="s">
         <v>433</v>
       </c>
-      <c r="E93" s="113" t="s">
+      <c r="E93" s="168" t="s">
         <v>434</v>
       </c>
-      <c r="F93" s="114"/>
+      <c r="F93" s="169"/>
     </row>
     <row r="94" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="118"/>
-      <c r="B94" s="120"/>
-      <c r="C94" s="120"/>
-      <c r="D94" s="120"/>
-      <c r="E94" s="115"/>
-      <c r="F94" s="116"/>
+      <c r="A94" s="137"/>
+      <c r="B94" s="138"/>
+      <c r="C94" s="138"/>
+      <c r="D94" s="138"/>
+      <c r="E94" s="170"/>
+      <c r="F94" s="171"/>
     </row>
     <row r="95" spans="1:7" ht="29.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="117" t="s">
+      <c r="A95" s="113" t="s">
         <v>435</v>
       </c>
-      <c r="B95" s="119" t="s">
+      <c r="B95" s="115" t="s">
         <v>436</v>
       </c>
-      <c r="C95" s="119" t="s">
+      <c r="C95" s="115" t="s">
         <v>437</v>
       </c>
-      <c r="D95" s="119" t="s">
+      <c r="D95" s="115" t="s">
         <v>438</v>
       </c>
       <c r="E95" s="72" t="s">
@@ -7639,10 +7639,10 @@
       <c r="F95" s="73"/>
     </row>
     <row r="96" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="118"/>
-      <c r="B96" s="120"/>
-      <c r="C96" s="120"/>
-      <c r="D96" s="120"/>
+      <c r="A96" s="137"/>
+      <c r="B96" s="138"/>
+      <c r="C96" s="138"/>
+      <c r="D96" s="138"/>
       <c r="E96" s="74" t="s">
         <v>440</v>
       </c>
@@ -7669,16 +7669,16 @@
       </c>
     </row>
     <row r="98" spans="1:6" ht="43.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="127" t="s">
+      <c r="A98" s="149" t="s">
         <v>420</v>
       </c>
-      <c r="B98" s="129" t="s">
+      <c r="B98" s="163" t="s">
         <v>325</v>
       </c>
-      <c r="C98" s="131">
-        <v>0</v>
-      </c>
-      <c r="D98" s="133">
+      <c r="C98" s="151">
+        <v>0</v>
+      </c>
+      <c r="D98" s="166">
         <v>100</v>
       </c>
       <c r="E98" s="57" t="s">
@@ -7689,34 +7689,34 @@
       </c>
     </row>
     <row r="99" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="128"/>
-      <c r="B99" s="130"/>
-      <c r="C99" s="132"/>
-      <c r="D99" s="134"/>
+      <c r="A99" s="162"/>
+      <c r="B99" s="164"/>
+      <c r="C99" s="165"/>
+      <c r="D99" s="167"/>
       <c r="E99" s="65"/>
       <c r="F99" s="66"/>
     </row>
     <row r="100" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="121" t="s">
+      <c r="A100" s="156" t="s">
         <v>422</v>
       </c>
-      <c r="B100" s="121" t="s">
+      <c r="B100" s="156" t="s">
         <v>423</v>
       </c>
-      <c r="C100" s="123">
-        <v>0</v>
-      </c>
-      <c r="D100" s="125">
+      <c r="C100" s="158">
+        <v>0</v>
+      </c>
+      <c r="D100" s="160">
         <v>50</v>
       </c>
       <c r="E100" s="57"/>
       <c r="F100" s="58"/>
     </row>
     <row r="101" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="122"/>
-      <c r="B101" s="122"/>
-      <c r="C101" s="124"/>
-      <c r="D101" s="126"/>
+      <c r="A101" s="157"/>
+      <c r="B101" s="157"/>
+      <c r="C101" s="159"/>
+      <c r="D101" s="161"/>
       <c r="E101" s="67" t="s">
         <v>424</v>
       </c>
@@ -7737,6 +7737,52 @@
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="E93:F94"/>
+    <mergeCell ref="A95:A96"/>
+    <mergeCell ref="B95:B96"/>
+    <mergeCell ref="C95:C96"/>
+    <mergeCell ref="D95:D96"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="C93:C94"/>
+    <mergeCell ref="D93:D94"/>
+    <mergeCell ref="A100:A101"/>
+    <mergeCell ref="B100:B101"/>
+    <mergeCell ref="C100:C101"/>
+    <mergeCell ref="D100:D101"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="B98:B99"/>
+    <mergeCell ref="C98:C99"/>
+    <mergeCell ref="D98:D99"/>
+    <mergeCell ref="A87:A91"/>
+    <mergeCell ref="B87:B91"/>
+    <mergeCell ref="C87:C91"/>
+    <mergeCell ref="D87:D91"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="B82:B86"/>
+    <mergeCell ref="C82:C86"/>
+    <mergeCell ref="D82:D86"/>
+    <mergeCell ref="A79:A81"/>
+    <mergeCell ref="B79:B81"/>
+    <mergeCell ref="C79:C81"/>
+    <mergeCell ref="D79:D81"/>
+    <mergeCell ref="A76:A78"/>
+    <mergeCell ref="B76:B78"/>
+    <mergeCell ref="C76:C78"/>
+    <mergeCell ref="D76:D78"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="A66:A75"/>
+    <mergeCell ref="B66:B75"/>
+    <mergeCell ref="C66:C75"/>
+    <mergeCell ref="D66:D75"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B40:B64"/>
+    <mergeCell ref="C40:C64"/>
+    <mergeCell ref="D40:D64"/>
+    <mergeCell ref="A9:A39"/>
+    <mergeCell ref="B9:B39"/>
+    <mergeCell ref="C9:C39"/>
+    <mergeCell ref="D9:D39"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="C6:C8"/>
@@ -7746,52 +7792,6 @@
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B40:B64"/>
-    <mergeCell ref="C40:C64"/>
-    <mergeCell ref="D40:D64"/>
-    <mergeCell ref="A9:A39"/>
-    <mergeCell ref="B9:B39"/>
-    <mergeCell ref="C9:C39"/>
-    <mergeCell ref="D9:D39"/>
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="A66:A75"/>
-    <mergeCell ref="B66:B75"/>
-    <mergeCell ref="C66:C75"/>
-    <mergeCell ref="D66:D75"/>
-    <mergeCell ref="A79:A81"/>
-    <mergeCell ref="B79:B81"/>
-    <mergeCell ref="C79:C81"/>
-    <mergeCell ref="D79:D81"/>
-    <mergeCell ref="A76:A78"/>
-    <mergeCell ref="B76:B78"/>
-    <mergeCell ref="C76:C78"/>
-    <mergeCell ref="D76:D78"/>
-    <mergeCell ref="A87:A91"/>
-    <mergeCell ref="B87:B91"/>
-    <mergeCell ref="C87:C91"/>
-    <mergeCell ref="D87:D91"/>
-    <mergeCell ref="A82:A86"/>
-    <mergeCell ref="B82:B86"/>
-    <mergeCell ref="C82:C86"/>
-    <mergeCell ref="D82:D86"/>
-    <mergeCell ref="A100:A101"/>
-    <mergeCell ref="B100:B101"/>
-    <mergeCell ref="C100:C101"/>
-    <mergeCell ref="D100:D101"/>
-    <mergeCell ref="A98:A99"/>
-    <mergeCell ref="B98:B99"/>
-    <mergeCell ref="C98:C99"/>
-    <mergeCell ref="D98:D99"/>
-    <mergeCell ref="E93:F94"/>
-    <mergeCell ref="A95:A96"/>
-    <mergeCell ref="B95:B96"/>
-    <mergeCell ref="C95:C96"/>
-    <mergeCell ref="D95:D96"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="C93:C94"/>
-    <mergeCell ref="D93:D94"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8223,8 +8223,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8504,7 +8504,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>

</xml_diff>